<commit_message>
Add copying of subject name and site to results, improve comments
</commit_message>
<xml_diff>
--- a/data/subject_results/Blank-Results.xlsx
+++ b/data/subject_results/Blank-Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sci-lmw1/dev/HelpLindsay/data/subject_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996CB845-5584-7B41-86C1-1B15417CF71B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C627DACD-3018-F243-B72A-52312B51CE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="519" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="519" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StudentOne" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
     <t xml:space="preserve">FORMAT STUDY_PACKAGE_RESULT STANDARD </t>
   </si>
@@ -256,9 +256,6 @@
   </si>
   <si>
     <t>KU</t>
-  </si>
-  <si>
-    <t>Problem Solving &amp; Programming 1</t>
   </si>
 </sst>
 </file>
@@ -5344,7 +5341,7 @@
       <pane xSplit="4" ySplit="12" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5372,9 +5369,7 @@
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="75" t="s">
-        <v>75</v>
-      </c>
+      <c r="C1" s="75"/>
       <c r="D1" s="50" t="s">
         <v>16</v>
       </c>
@@ -19516,21 +19511,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060D23BF17FCDC947B8E404D646247F8D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f8a301bd3e0c8b5ed750a66ab7022">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0f5e39c8-e5a1-4a0d-b53f-9134be983d19" xmlns:ns3="c64b295e-e158-430a-a9fe-95bbf17b9d7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="765cdbe449e857445462344bdfd818c7" ns2:_="" ns3:_="">
     <xsd:import namespace="0f5e39c8-e5a1-4a0d-b53f-9134be983d19"/>
@@ -19747,10 +19727,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB09DFA-8D31-49CC-B484-1597D6808628}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A6C0948-47EA-46A4-908A-6D65E67CB754}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0f5e39c8-e5a1-4a0d-b53f-9134be983d19"/>
+    <ds:schemaRef ds:uri="c64b295e-e158-430a-a9fe-95bbf17b9d7d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19773,20 +19779,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A6C0948-47EA-46A4-908A-6D65E67CB754}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB09DFA-8D31-49CC-B484-1597D6808628}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0f5e39c8-e5a1-4a0d-b53f-9134be983d19"/>
-    <ds:schemaRef ds:uri="c64b295e-e158-430a-a9fe-95bbf17b9d7d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add setting of subject and site in StudentOne sheet
</commit_message>
<xml_diff>
--- a/data/subject_results/Blank-Results.xlsx
+++ b/data/subject_results/Blank-Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sci-lmw1/dev/HelpLindsay/data/subject_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C627DACD-3018-F243-B72A-52312B51CE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBD39BC-EAEC-4344-99F3-C20123EE16FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="519" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="519" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StudentOne" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t xml:space="preserve">FORMAT STUDY_PACKAGE_RESULT STANDARD </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Parent Ssp No</t>
   </si>
   <si>
     <t>Parent Spk Cd</t>
@@ -82,9 +79,6 @@
   </si>
   <si>
     <t>Grade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mark </t>
   </si>
   <si>
     <t>Subject Name</t>
@@ -256,6 +250,9 @@
   </si>
   <si>
     <t>KU</t>
+  </si>
+  <si>
+    <t>Parent Ssp No</t>
   </si>
 </sst>
 </file>
@@ -628,7 +625,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1041,34 +1038,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1117,7 +1086,7 @@
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -1290,14 +1259,6 @@
     <xf numFmtId="2" fontId="0" fillId="32" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1312,6 +1273,13 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2212,3094 +2180,3092 @@
   </sheetPr>
   <dimension ref="A1:Q503"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="14" width="9.1640625" style="67"/>
-    <col min="15" max="15" width="22.1640625" style="67" customWidth="1"/>
-    <col min="16" max="16" width="9.1640625" style="68"/>
-    <col min="17" max="16384" width="9.1640625" style="67"/>
+    <col min="1" max="14" width="9.1640625" style="74"/>
+    <col min="15" max="15" width="22.1640625" style="74" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="72"/>
+    <col min="17" max="16384" width="9.1640625" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="Q1" s="68"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="Q1" s="72"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="C2" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="D2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="E2" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="F2" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="G2" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="H2" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="I2" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="J2" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="68" t="s">
+      <c r="K2" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="68" t="s">
+      <c r="L2" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="68" t="s">
+      <c r="M2" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="68" t="s">
+      <c r="N2" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="68" t="s">
+      <c r="O2" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="68" t="s">
+      <c r="P2" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="68" t="s">
-        <v>17</v>
-      </c>
+      <c r="Q2" s="72"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P3" s="69" t="str">
+      <c r="P3" s="72" t="str">
         <f>IF($N3="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N3,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N3,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P4" s="69" t="str">
+      <c r="P4" s="72" t="str">
         <f>IF($N4="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N4,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N4,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P5" s="69" t="str">
+      <c r="P5" s="72" t="str">
         <f>IF($N5="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N5,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N5,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P6" s="69" t="str">
+      <c r="P6" s="72" t="str">
         <f>IF($N6="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N6,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N6,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P7" s="69" t="str">
+      <c r="P7" s="72" t="str">
         <f>IF($N7="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N7,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N7,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P8" s="69" t="str">
+      <c r="P8" s="72" t="str">
         <f>IF($N8="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N8,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N8,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P9" s="69" t="str">
+      <c r="P9" s="72" t="str">
         <f>IF($N9="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N9,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N9,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P10" s="69" t="str">
+      <c r="P10" s="72" t="str">
         <f>IF($N10="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N10,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N10,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P11" s="69" t="str">
+      <c r="P11" s="72" t="str">
         <f>IF($N11="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N11,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N11,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P12" s="69" t="str">
+      <c r="P12" s="72" t="str">
         <f>IF($N12="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N12,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N12,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P13" s="69" t="str">
+      <c r="P13" s="72" t="str">
         <f>IF($N13="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N13,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N13,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P14" s="69" t="str">
+      <c r="P14" s="72" t="str">
         <f>IF($N14="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N14,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N14,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P15" s="69" t="str">
+      <c r="P15" s="72" t="str">
         <f>IF($N15="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N15,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N15,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="P16" s="69" t="str">
+      <c r="P16" s="72" t="str">
         <f>IF($N16="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N16,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N16,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P17" s="69" t="str">
+      <c r="P17" s="72" t="str">
         <f>IF($N17="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N17,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N17,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P18" s="69" t="str">
+      <c r="P18" s="72" t="str">
         <f>IF($N18="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N18,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N18,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P19" s="69" t="str">
+      <c r="P19" s="72" t="str">
         <f>IF($N19="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N19,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N19,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P20" s="69" t="str">
+      <c r="P20" s="72" t="str">
         <f>IF($N20="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N20,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N20,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P21" s="69" t="str">
+      <c r="P21" s="72" t="str">
         <f>IF($N21="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N21,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N21,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P22" s="69" t="str">
+      <c r="P22" s="72" t="str">
         <f>IF($N22="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N22,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N22,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P23" s="69" t="str">
+      <c r="P23" s="72" t="str">
         <f>IF($N23="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N23,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N23,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P24" s="69" t="str">
+      <c r="P24" s="72" t="str">
         <f>IF($N24="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N24,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N24,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P25" s="69" t="str">
+      <c r="P25" s="72" t="str">
         <f>IF($N25="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N25,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N25,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P26" s="69" t="str">
+      <c r="P26" s="72" t="str">
         <f>IF($N26="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N26,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N26,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P27" s="69" t="str">
+      <c r="P27" s="72" t="str">
         <f>IF($N27="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N27,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N27,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P28" s="69" t="str">
+      <c r="P28" s="72" t="str">
         <f>IF($N28="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N28,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N28,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P29" s="69" t="str">
+      <c r="P29" s="72" t="str">
         <f>IF($N29="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N29,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N29,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P30" s="69" t="str">
+      <c r="P30" s="72" t="str">
         <f>IF($N30="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N30,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N30,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P31" s="69" t="str">
+      <c r="P31" s="72" t="str">
         <f>IF($N31="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N31,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N31,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P32" s="69" t="str">
+      <c r="P32" s="72" t="str">
         <f>IF($N32="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N32,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N32,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P33" s="69" t="str">
+      <c r="P33" s="72" t="str">
         <f>IF($N33="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N33,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N33,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P34" s="69" t="str">
+      <c r="P34" s="72" t="str">
         <f>IF($N34="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N34,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N34,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P35" s="69" t="str">
+      <c r="P35" s="72" t="str">
         <f>IF($N35="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N35,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N35,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P36" s="69" t="str">
+      <c r="P36" s="72" t="str">
         <f>IF($N36="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N36,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N36,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P37" s="69" t="str">
+      <c r="P37" s="72" t="str">
         <f>IF($N37="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N37,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N37,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P38" s="69" t="str">
+      <c r="P38" s="72" t="str">
         <f>IF($N38="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N38,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N38,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P39" s="69" t="str">
+      <c r="P39" s="72" t="str">
         <f>IF($N39="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N39,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N39,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P40" s="69" t="str">
+      <c r="P40" s="72" t="str">
         <f>IF($N40="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N40,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N40,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P41" s="69" t="str">
+      <c r="P41" s="72" t="str">
         <f>IF($N41="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N41,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N41,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P42" s="69" t="str">
+      <c r="P42" s="72" t="str">
         <f>IF($N42="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N42,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N42,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P43" s="69" t="str">
+      <c r="P43" s="72" t="str">
         <f>IF($N43="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N43,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N43,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P44" s="69" t="str">
+      <c r="P44" s="72" t="str">
         <f>IF($N44="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N44,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N44,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P45" s="69" t="str">
+      <c r="P45" s="72" t="str">
         <f>IF($N45="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N45,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N45,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P46" s="69" t="str">
+      <c r="P46" s="72" t="str">
         <f>IF($N46="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N46,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N46,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P47" s="69" t="str">
+      <c r="P47" s="72" t="str">
         <f>IF($N47="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N47,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N47,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P48" s="69" t="str">
+      <c r="P48" s="72" t="str">
         <f>IF($N48="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N48,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N48,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P49" s="69" t="str">
+      <c r="P49" s="72" t="str">
         <f>IF($N49="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N49,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N49,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P50" s="69" t="str">
+      <c r="P50" s="72" t="str">
         <f>IF($N50="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N50,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N50,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P51" s="69" t="str">
+      <c r="P51" s="72" t="str">
         <f>IF($N51="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N51,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N51,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P52" s="69" t="str">
+      <c r="P52" s="72" t="str">
         <f>IF($N52="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N52,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N52,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P53" s="69" t="str">
+      <c r="P53" s="72" t="str">
         <f>IF($N53="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N53,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N53,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P54" s="69" t="str">
+      <c r="P54" s="72" t="str">
         <f>IF($N54="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N54,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N54,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P55" s="69" t="str">
+      <c r="P55" s="72" t="str">
         <f>IF($N55="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N55,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N55,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P56" s="69" t="str">
+      <c r="P56" s="72" t="str">
         <f>IF($N56="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N56,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N56,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="57" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P57" s="69" t="str">
+      <c r="P57" s="72" t="str">
         <f>IF($N57="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N57,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N57,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="58" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P58" s="69" t="str">
+      <c r="P58" s="72" t="str">
         <f>IF($N58="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N58,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N58,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="59" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P59" s="69" t="str">
+      <c r="P59" s="72" t="str">
         <f>IF($N59="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N59,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N59,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="60" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P60" s="69" t="str">
+      <c r="P60" s="72" t="str">
         <f>IF($N60="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N60,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N60,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="61" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P61" s="69" t="str">
+      <c r="P61" s="72" t="str">
         <f>IF($N61="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N61,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N61,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="62" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P62" s="69" t="str">
+      <c r="P62" s="72" t="str">
         <f>IF($N62="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N62,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N62,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="63" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P63" s="69" t="str">
+      <c r="P63" s="72" t="str">
         <f>IF($N63="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N63,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N63,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="64" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P64" s="69" t="str">
+      <c r="P64" s="72" t="str">
         <f>IF($N64="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N64,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N64,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="65" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P65" s="69" t="str">
+      <c r="P65" s="72" t="str">
         <f>IF($N65="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N65,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N65,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="66" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P66" s="69" t="str">
+      <c r="P66" s="72" t="str">
         <f>IF($N66="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N66,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N66,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P67" s="69" t="str">
+      <c r="P67" s="72" t="str">
         <f>IF($N67="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N67,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N67,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P68" s="69" t="str">
+      <c r="P68" s="72" t="str">
         <f>IF($N68="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N68,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N68,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="69" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P69" s="69" t="str">
+      <c r="P69" s="72" t="str">
         <f>IF($N69="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N69,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N69,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="70" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P70" s="69" t="str">
+      <c r="P70" s="72" t="str">
         <f>IF($N70="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N70,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N70,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="71" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P71" s="69" t="str">
+      <c r="P71" s="72" t="str">
         <f>IF($N71="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N71,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N71,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P72" s="69" t="str">
+      <c r="P72" s="72" t="str">
         <f>IF($N72="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N72,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N72,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="73" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P73" s="69" t="str">
+      <c r="P73" s="72" t="str">
         <f>IF($N73="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N73,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N73,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="74" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P74" s="69" t="str">
+      <c r="P74" s="72" t="str">
         <f>IF($N74="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N74,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N74,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="75" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P75" s="69" t="str">
+      <c r="P75" s="72" t="str">
         <f>IF($N75="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N75,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N75,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P76" s="69" t="str">
+      <c r="P76" s="72" t="str">
         <f>IF($N76="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N76,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N76,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="77" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P77" s="69" t="str">
+      <c r="P77" s="72" t="str">
         <f>IF($N77="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N77,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N77,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="78" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P78" s="69" t="str">
+      <c r="P78" s="72" t="str">
         <f>IF($N78="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N78,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N78,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="79" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P79" s="69" t="str">
+      <c r="P79" s="72" t="str">
         <f>IF($N79="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N79,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N79,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="80" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P80" s="69" t="str">
+      <c r="P80" s="72" t="str">
         <f>IF($N80="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N80,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N80,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="81" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P81" s="69" t="str">
+      <c r="P81" s="72" t="str">
         <f>IF($N81="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N81,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N81,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="82" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P82" s="69" t="str">
+      <c r="P82" s="72" t="str">
         <f>IF($N82="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N82,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N82,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="83" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P83" s="69" t="str">
+      <c r="P83" s="72" t="str">
         <f>IF($N83="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N83,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N83,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="84" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P84" s="69" t="str">
+      <c r="P84" s="72" t="str">
         <f>IF($N84="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N84,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N84,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="85" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P85" s="69" t="str">
+      <c r="P85" s="72" t="str">
         <f>IF($N85="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N85,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N85,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="86" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P86" s="69" t="str">
+      <c r="P86" s="72" t="str">
         <f>IF($N86="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N86,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N86,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="87" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P87" s="69" t="str">
+      <c r="P87" s="72" t="str">
         <f>IF($N87="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N87,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N87,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="88" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P88" s="69" t="str">
+      <c r="P88" s="72" t="str">
         <f>IF($N88="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N88,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N88,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="89" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P89" s="69" t="str">
+      <c r="P89" s="72" t="str">
         <f>IF($N89="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N89,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N89,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="90" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P90" s="69" t="str">
+      <c r="P90" s="72" t="str">
         <f>IF($N90="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N90,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N90,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="91" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P91" s="69" t="str">
+      <c r="P91" s="72" t="str">
         <f>IF($N91="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N91,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N91,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="92" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P92" s="69" t="str">
+      <c r="P92" s="72" t="str">
         <f>IF($N92="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N92,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N92,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="93" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P93" s="69" t="str">
+      <c r="P93" s="72" t="str">
         <f>IF($N93="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N93,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N93,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="94" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P94" s="69" t="str">
+      <c r="P94" s="72" t="str">
         <f>IF($N94="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N94,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N94,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="95" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P95" s="69" t="str">
+      <c r="P95" s="72" t="str">
         <f>IF($N95="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N95,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N95,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="96" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P96" s="69" t="str">
+      <c r="P96" s="72" t="str">
         <f>IF($N96="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N96,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N96,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="97" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P97" s="69" t="str">
+      <c r="P97" s="72" t="str">
         <f>IF($N97="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N97,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N97,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="98" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P98" s="69" t="str">
+      <c r="P98" s="72" t="str">
         <f>IF($N98="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N98,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N98,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="99" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P99" s="69" t="str">
+      <c r="P99" s="72" t="str">
         <f>IF($N99="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N99,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N99,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="100" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P100" s="69" t="str">
+      <c r="P100" s="72" t="str">
         <f>IF($N100="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N100,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N100,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="101" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P101" s="69" t="str">
+      <c r="P101" s="72" t="str">
         <f>IF($N101="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N101,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N101,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="102" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P102" s="69" t="str">
+      <c r="P102" s="72" t="str">
         <f>IF($N102="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N102,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N102,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="103" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P103" s="69" t="str">
+      <c r="P103" s="72" t="str">
         <f>IF($N103="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N103,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N103,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="104" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P104" s="69" t="str">
+      <c r="P104" s="72" t="str">
         <f>IF($N104="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N104,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N104,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="105" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P105" s="69" t="str">
+      <c r="P105" s="72" t="str">
         <f>IF($N105="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N105,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N105,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="106" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P106" s="69" t="str">
+      <c r="P106" s="72" t="str">
         <f>IF($N106="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N106,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N106,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="107" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P107" s="69" t="str">
+      <c r="P107" s="72" t="str">
         <f>IF($N107="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N107,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N107,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="108" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P108" s="69" t="str">
+      <c r="P108" s="72" t="str">
         <f>IF($N108="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N108,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N108,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="109" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P109" s="69" t="str">
+      <c r="P109" s="72" t="str">
         <f>IF($N109="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N109,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N109,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="110" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P110" s="69" t="str">
+      <c r="P110" s="72" t="str">
         <f>IF($N110="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N110,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N110,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="111" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P111" s="69" t="str">
+      <c r="P111" s="72" t="str">
         <f>IF($N111="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N111,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N111,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="112" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P112" s="69" t="str">
+      <c r="P112" s="72" t="str">
         <f>IF($N112="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N112,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N112,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="113" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P113" s="69" t="str">
+      <c r="P113" s="72" t="str">
         <f>IF($N113="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N113,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N113,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="114" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P114" s="69" t="str">
+      <c r="P114" s="72" t="str">
         <f>IF($N114="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N114,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N114,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="115" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P115" s="69" t="str">
+      <c r="P115" s="72" t="str">
         <f>IF($N115="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N115,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N115,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="116" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P116" s="69" t="str">
+      <c r="P116" s="72" t="str">
         <f>IF($N116="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N116,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N116,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="117" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P117" s="69" t="str">
+      <c r="P117" s="72" t="str">
         <f>IF($N117="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N117,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N117,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="118" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P118" s="69" t="str">
+      <c r="P118" s="72" t="str">
         <f>IF($N118="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N118,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N118,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="119" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P119" s="69" t="str">
+      <c r="P119" s="72" t="str">
         <f>IF($N119="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N119,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N119,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="120" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P120" s="69" t="str">
+      <c r="P120" s="72" t="str">
         <f>IF($N120="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N120,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N120,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="121" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P121" s="69" t="str">
+      <c r="P121" s="72" t="str">
         <f>IF($N121="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N121,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N121,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="122" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P122" s="69" t="str">
+      <c r="P122" s="72" t="str">
         <f>IF($N122="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N122,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N122,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="123" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P123" s="69" t="str">
+      <c r="P123" s="72" t="str">
         <f>IF($N123="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N123,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N123,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="124" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P124" s="69" t="str">
+      <c r="P124" s="72" t="str">
         <f>IF($N124="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N124,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N124,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="125" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P125" s="69" t="str">
+      <c r="P125" s="72" t="str">
         <f>IF($N125="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N125,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N125,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="126" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P126" s="69" t="str">
+      <c r="P126" s="72" t="str">
         <f>IF($N126="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N126,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N126,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="127" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P127" s="69" t="str">
+      <c r="P127" s="72" t="str">
         <f>IF($N127="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N127,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N127,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="128" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P128" s="69" t="str">
+      <c r="P128" s="72" t="str">
         <f>IF($N128="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N128,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N128,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="129" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P129" s="69" t="str">
+      <c r="P129" s="72" t="str">
         <f>IF($N129="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N129,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N129,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="130" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P130" s="69" t="str">
+      <c r="P130" s="72" t="str">
         <f>IF($N130="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N130,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N130,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="131" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P131" s="69" t="str">
+      <c r="P131" s="72" t="str">
         <f>IF($N131="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N131,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N131,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="132" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P132" s="69" t="str">
+      <c r="P132" s="72" t="str">
         <f>IF($N132="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N132,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N132,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="133" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P133" s="69" t="str">
+      <c r="P133" s="72" t="str">
         <f>IF($N133="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N133,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N133,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="134" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P134" s="69" t="str">
+      <c r="P134" s="72" t="str">
         <f>IF($N134="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N134,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N134,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="135" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P135" s="69" t="str">
+      <c r="P135" s="72" t="str">
         <f>IF($N135="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N135,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N135,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="136" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P136" s="69" t="str">
+      <c r="P136" s="72" t="str">
         <f>IF($N136="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N136,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N136,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="137" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P137" s="69" t="str">
+      <c r="P137" s="72" t="str">
         <f>IF($N137="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N137,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N137,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="138" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P138" s="69" t="str">
+      <c r="P138" s="72" t="str">
         <f>IF($N138="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N138,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N138,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="139" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P139" s="69" t="str">
+      <c r="P139" s="72" t="str">
         <f>IF($N139="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N139,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N139,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="140" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P140" s="69" t="str">
+      <c r="P140" s="72" t="str">
         <f>IF($N140="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N140,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N140,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="141" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P141" s="69" t="str">
+      <c r="P141" s="72" t="str">
         <f>IF($N141="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N141,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N141,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="142" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P142" s="69" t="str">
+      <c r="P142" s="72" t="str">
         <f>IF($N142="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N142,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N142,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="143" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P143" s="69" t="str">
+      <c r="P143" s="72" t="str">
         <f>IF($N143="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N143,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N143,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="144" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P144" s="69" t="str">
+      <c r="P144" s="72" t="str">
         <f>IF($N144="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N144,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N144,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="145" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P145" s="69" t="str">
+      <c r="P145" s="72" t="str">
         <f>IF($N145="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N145,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N145,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="146" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P146" s="69" t="str">
+      <c r="P146" s="72" t="str">
         <f>IF($N146="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N146,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N146,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="147" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P147" s="69" t="str">
+      <c r="P147" s="72" t="str">
         <f>IF($N147="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N147,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N147,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="148" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P148" s="69" t="str">
+      <c r="P148" s="72" t="str">
         <f>IF($N148="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N148,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N148,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="149" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P149" s="69" t="str">
+      <c r="P149" s="72" t="str">
         <f>IF($N149="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N149,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N149,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="150" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P150" s="69" t="str">
+      <c r="P150" s="72" t="str">
         <f>IF($N150="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N150,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N150,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="151" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P151" s="69" t="str">
+      <c r="P151" s="72" t="str">
         <f>IF($N151="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N151,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N151,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="152" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P152" s="69" t="str">
+      <c r="P152" s="72" t="str">
         <f>IF($N152="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N152,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N152,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="153" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P153" s="69" t="str">
+      <c r="P153" s="72" t="str">
         <f>IF($N153="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N153,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N153,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="154" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P154" s="69" t="str">
+      <c r="P154" s="72" t="str">
         <f>IF($N154="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N154,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N154,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="155" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P155" s="69" t="str">
+      <c r="P155" s="72" t="str">
         <f>IF($N155="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N155,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N155,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="156" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P156" s="69" t="str">
+      <c r="P156" s="72" t="str">
         <f>IF($N156="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N156,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N156,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="157" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P157" s="69" t="str">
+      <c r="P157" s="72" t="str">
         <f>IF($N157="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N157,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N157,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="158" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P158" s="69" t="str">
+      <c r="P158" s="72" t="str">
         <f>IF($N158="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N158,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N158,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="159" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P159" s="69" t="str">
+      <c r="P159" s="72" t="str">
         <f>IF($N159="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N159,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N159,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="160" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P160" s="69" t="str">
+      <c r="P160" s="72" t="str">
         <f>IF($N160="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N160,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N160,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="161" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P161" s="69" t="str">
+      <c r="P161" s="72" t="str">
         <f>IF($N161="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N161,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N161,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="162" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P162" s="69" t="str">
+      <c r="P162" s="72" t="str">
         <f>IF($N162="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N162,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N162,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="163" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P163" s="69" t="str">
+      <c r="P163" s="72" t="str">
         <f>IF($N163="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N163,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N163,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="164" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P164" s="69" t="str">
+      <c r="P164" s="72" t="str">
         <f>IF($N164="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N164,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N164,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="165" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P165" s="69" t="str">
+      <c r="P165" s="72" t="str">
         <f>IF($N165="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N165,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N165,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="166" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P166" s="69" t="str">
+      <c r="P166" s="72" t="str">
         <f>IF($N166="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N166,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N166,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="167" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P167" s="69" t="str">
+      <c r="P167" s="72" t="str">
         <f>IF($N167="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N167,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N167,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="168" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P168" s="69" t="str">
+      <c r="P168" s="72" t="str">
         <f>IF($N168="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N168,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N168,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="169" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P169" s="69" t="str">
+      <c r="P169" s="72" t="str">
         <f>IF($N169="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N169,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N169,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="170" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P170" s="69" t="str">
+      <c r="P170" s="72" t="str">
         <f>IF($N170="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N170,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N170,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="171" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P171" s="69" t="str">
+      <c r="P171" s="72" t="str">
         <f>IF($N171="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N171,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N171,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="172" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P172" s="69" t="str">
+      <c r="P172" s="72" t="str">
         <f>IF($N172="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N172,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N172,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="173" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P173" s="69" t="str">
+      <c r="P173" s="72" t="str">
         <f>IF($N173="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N173,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N173,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="174" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P174" s="69" t="str">
+      <c r="P174" s="72" t="str">
         <f>IF($N174="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N174,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N174,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="175" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P175" s="69" t="str">
+      <c r="P175" s="72" t="str">
         <f>IF($N175="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N175,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N175,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="176" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P176" s="69" t="str">
+      <c r="P176" s="72" t="str">
         <f>IF($N176="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N176,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N176,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="177" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P177" s="69" t="str">
+      <c r="P177" s="72" t="str">
         <f>IF($N177="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N177,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N177,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="178" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P178" s="69" t="str">
+      <c r="P178" s="72" t="str">
         <f>IF($N178="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N178,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N178,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="179" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P179" s="69" t="str">
+      <c r="P179" s="72" t="str">
         <f>IF($N179="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N179,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N179,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="180" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P180" s="69" t="str">
+      <c r="P180" s="72" t="str">
         <f>IF($N180="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N180,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N180,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="181" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P181" s="69" t="str">
+      <c r="P181" s="72" t="str">
         <f>IF($N181="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N181,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N181,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="182" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P182" s="69" t="str">
+      <c r="P182" s="72" t="str">
         <f>IF($N182="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N182,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N182,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="183" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P183" s="69" t="str">
+      <c r="P183" s="72" t="str">
         <f>IF($N183="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N183,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N183,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="184" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P184" s="69" t="str">
+      <c r="P184" s="72" t="str">
         <f>IF($N184="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N184,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N184,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="185" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P185" s="69" t="str">
+      <c r="P185" s="72" t="str">
         <f>IF($N185="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N185,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N185,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="186" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P186" s="69" t="str">
+      <c r="P186" s="72" t="str">
         <f>IF($N186="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N186,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N186,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="187" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P187" s="69" t="str">
+      <c r="P187" s="72" t="str">
         <f>IF($N187="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N187,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N187,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="188" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P188" s="69" t="str">
+      <c r="P188" s="72" t="str">
         <f>IF($N188="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N188,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N188,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="189" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P189" s="69" t="str">
+      <c r="P189" s="72" t="str">
         <f>IF($N189="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N189,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N189,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="190" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P190" s="69" t="str">
+      <c r="P190" s="72" t="str">
         <f>IF($N190="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N190,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N190,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="191" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P191" s="69" t="str">
+      <c r="P191" s="72" t="str">
         <f>IF($N191="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N191,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N191,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="192" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P192" s="69" t="str">
+      <c r="P192" s="72" t="str">
         <f>IF($N192="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N192,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N192,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="193" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P193" s="69" t="str">
+      <c r="P193" s="72" t="str">
         <f>IF($N193="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N193,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N193,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="194" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P194" s="69" t="str">
+      <c r="P194" s="72" t="str">
         <f>IF($N194="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N194,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N194,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="195" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P195" s="69" t="str">
+      <c r="P195" s="72" t="str">
         <f>IF($N195="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N195,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N195,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="196" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P196" s="69" t="str">
+      <c r="P196" s="72" t="str">
         <f>IF($N196="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N196,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N196,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="197" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P197" s="69" t="str">
+      <c r="P197" s="72" t="str">
         <f>IF($N197="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N197,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N197,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="198" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P198" s="69" t="str">
+      <c r="P198" s="72" t="str">
         <f>IF($N198="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N198,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N198,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="199" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P199" s="69" t="str">
+      <c r="P199" s="72" t="str">
         <f>IF($N199="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N199,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N199,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="200" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P200" s="69" t="str">
+      <c r="P200" s="72" t="str">
         <f>IF($N200="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N200,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N200,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="201" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P201" s="69" t="str">
+      <c r="P201" s="72" t="str">
         <f>IF($N201="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N201,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N201,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="202" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P202" s="69" t="str">
+      <c r="P202" s="72" t="str">
         <f>IF($N202="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N202,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N202,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="203" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P203" s="69" t="str">
+      <c r="P203" s="72" t="str">
         <f>IF($N203="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N203,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N203,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="204" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P204" s="69" t="str">
+      <c r="P204" s="72" t="str">
         <f>IF($N204="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N204,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N204,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="205" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P205" s="69" t="str">
+      <c r="P205" s="72" t="str">
         <f>IF($N205="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N205,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N205,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="206" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P206" s="69" t="str">
+      <c r="P206" s="72" t="str">
         <f>IF($N206="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N206,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N206,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="207" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P207" s="69" t="str">
+      <c r="P207" s="72" t="str">
         <f>IF($N207="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N207,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N207,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="208" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P208" s="69" t="str">
+      <c r="P208" s="72" t="str">
         <f>IF($N208="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N208,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N208,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="209" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P209" s="69" t="str">
+      <c r="P209" s="72" t="str">
         <f>IF($N209="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N209,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N209,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="210" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P210" s="69" t="str">
+      <c r="P210" s="72" t="str">
         <f>IF($N210="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N210,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N210,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="211" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P211" s="69" t="str">
+      <c r="P211" s="72" t="str">
         <f>IF($N211="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N211,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N211,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="212" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P212" s="69" t="str">
+      <c r="P212" s="72" t="str">
         <f>IF($N212="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N212,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N212,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="213" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P213" s="69" t="str">
+      <c r="P213" s="72" t="str">
         <f>IF($N213="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N213,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N213,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="214" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P214" s="69" t="str">
+      <c r="P214" s="72" t="str">
         <f>IF($N214="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N214,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N214,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="215" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P215" s="69" t="str">
+      <c r="P215" s="72" t="str">
         <f>IF($N215="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N215,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N215,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="216" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P216" s="69" t="str">
+      <c r="P216" s="72" t="str">
         <f>IF($N216="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N216,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N216,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="217" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P217" s="69" t="str">
+      <c r="P217" s="72" t="str">
         <f>IF($N217="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N217,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N217,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="218" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P218" s="69" t="str">
+      <c r="P218" s="72" t="str">
         <f>IF($N218="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N218,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N218,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="219" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P219" s="69" t="str">
+      <c r="P219" s="72" t="str">
         <f>IF($N219="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N219,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N219,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="220" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P220" s="69" t="str">
+      <c r="P220" s="72" t="str">
         <f>IF($N220="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N220,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N220,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="221" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P221" s="69" t="str">
+      <c r="P221" s="72" t="str">
         <f>IF($N221="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N221,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N221,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="222" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P222" s="69" t="str">
+      <c r="P222" s="72" t="str">
         <f>IF($N222="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N222,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N222,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="223" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P223" s="69" t="str">
+      <c r="P223" s="72" t="str">
         <f>IF($N223="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N223,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N223,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="224" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P224" s="69" t="str">
+      <c r="P224" s="72" t="str">
         <f>IF($N224="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N224,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N224,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="225" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P225" s="69" t="str">
+      <c r="P225" s="72" t="str">
         <f>IF($N225="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N225,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N225,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="226" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P226" s="69" t="str">
+      <c r="P226" s="72" t="str">
         <f>IF($N226="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N226,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N226,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="227" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P227" s="69" t="str">
+      <c r="P227" s="72" t="str">
         <f>IF($N227="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N227,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N227,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="228" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P228" s="69" t="str">
+      <c r="P228" s="72" t="str">
         <f>IF($N228="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N228,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N228,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="229" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P229" s="69" t="str">
+      <c r="P229" s="72" t="str">
         <f>IF($N229="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N229,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N229,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="230" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P230" s="69" t="str">
+      <c r="P230" s="72" t="str">
         <f>IF($N230="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N230,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N230,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="231" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P231" s="69" t="str">
+      <c r="P231" s="72" t="str">
         <f>IF($N231="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N231,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N231,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="232" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P232" s="69" t="str">
+      <c r="P232" s="72" t="str">
         <f>IF($N232="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N232,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N232,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="233" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P233" s="69" t="str">
+      <c r="P233" s="72" t="str">
         <f>IF($N233="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N233,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N233,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="234" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P234" s="69" t="str">
+      <c r="P234" s="72" t="str">
         <f>IF($N234="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N234,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N234,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="235" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P235" s="69" t="str">
+      <c r="P235" s="72" t="str">
         <f>IF($N235="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N235,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N235,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="236" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P236" s="69" t="str">
+      <c r="P236" s="72" t="str">
         <f>IF($N236="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N236,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N236,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="237" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P237" s="69" t="str">
+      <c r="P237" s="72" t="str">
         <f>IF($N237="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N237,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N237,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="238" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P238" s="69" t="str">
+      <c r="P238" s="72" t="str">
         <f>IF($N238="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N238,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N238,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="239" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P239" s="69" t="str">
+      <c r="P239" s="72" t="str">
         <f>IF($N239="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N239,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N239,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="240" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P240" s="69" t="str">
+      <c r="P240" s="72" t="str">
         <f>IF($N240="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N240,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N240,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="241" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P241" s="69" t="str">
+      <c r="P241" s="72" t="str">
         <f>IF($N241="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N241,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N241,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="242" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P242" s="69" t="str">
+      <c r="P242" s="72" t="str">
         <f>IF($N242="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N242,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N242,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="243" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P243" s="69" t="str">
+      <c r="P243" s="72" t="str">
         <f>IF($N243="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N243,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N243,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="244" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P244" s="69" t="str">
+      <c r="P244" s="72" t="str">
         <f>IF($N244="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N244,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N244,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="245" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P245" s="69" t="str">
+      <c r="P245" s="72" t="str">
         <f>IF($N245="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N245,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N245,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="246" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P246" s="69" t="str">
+      <c r="P246" s="72" t="str">
         <f>IF($N246="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N246,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N246,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="247" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P247" s="69" t="str">
+      <c r="P247" s="72" t="str">
         <f>IF($N247="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N247,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N247,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="248" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P248" s="69" t="str">
+      <c r="P248" s="72" t="str">
         <f>IF($N248="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N248,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N248,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="249" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P249" s="69" t="str">
+      <c r="P249" s="72" t="str">
         <f>IF($N249="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N249,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N249,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="250" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P250" s="69" t="str">
+      <c r="P250" s="72" t="str">
         <f>IF($N250="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N250,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N250,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="251" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P251" s="69" t="str">
+      <c r="P251" s="72" t="str">
         <f>IF($N251="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N251,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N251,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="252" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P252" s="69" t="str">
+      <c r="P252" s="72" t="str">
         <f>IF($N252="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N252,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N252,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="253" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P253" s="69" t="str">
+      <c r="P253" s="72" t="str">
         <f>IF($N253="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N253,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N253,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="254" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P254" s="69" t="str">
+      <c r="P254" s="72" t="str">
         <f>IF($N254="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N254,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N254,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="255" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P255" s="69" t="str">
+      <c r="P255" s="72" t="str">
         <f>IF($N255="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N255,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N255,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="256" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P256" s="69" t="str">
+      <c r="P256" s="72" t="str">
         <f>IF($N256="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N256,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N256,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="257" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P257" s="69" t="str">
+      <c r="P257" s="72" t="str">
         <f>IF($N257="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N257,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N257,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="258" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P258" s="69" t="str">
+      <c r="P258" s="72" t="str">
         <f>IF($N258="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N258,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N258,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="259" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P259" s="69" t="str">
+      <c r="P259" s="72" t="str">
         <f>IF($N259="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N259,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N259,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="260" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P260" s="69" t="str">
+      <c r="P260" s="72" t="str">
         <f>IF($N260="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N260,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N260,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="261" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P261" s="69" t="str">
+      <c r="P261" s="72" t="str">
         <f>IF($N261="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N261,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N261,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="262" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P262" s="69" t="str">
+      <c r="P262" s="72" t="str">
         <f>IF($N262="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N262,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N262,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="263" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P263" s="69" t="str">
+      <c r="P263" s="72" t="str">
         <f>IF($N263="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N263,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N263,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="264" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P264" s="69" t="str">
+      <c r="P264" s="72" t="str">
         <f>IF($N264="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N264,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N264,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="265" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P265" s="69" t="str">
+      <c r="P265" s="72" t="str">
         <f>IF($N265="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N265,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N265,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="266" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P266" s="69" t="str">
+      <c r="P266" s="72" t="str">
         <f>IF($N266="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N266,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N266,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="267" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P267" s="69" t="str">
+      <c r="P267" s="72" t="str">
         <f>IF($N267="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N267,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N267,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="268" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P268" s="69" t="str">
+      <c r="P268" s="72" t="str">
         <f>IF($N268="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N268,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N268,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="269" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P269" s="69" t="str">
+      <c r="P269" s="72" t="str">
         <f>IF($N269="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N269,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N269,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="270" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P270" s="69" t="str">
+      <c r="P270" s="72" t="str">
         <f>IF($N270="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N270,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N270,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="271" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P271" s="69" t="str">
+      <c r="P271" s="72" t="str">
         <f>IF($N271="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N271,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N271,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="272" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P272" s="69" t="str">
+      <c r="P272" s="72" t="str">
         <f>IF($N272="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N272,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N272,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="273" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P273" s="69" t="str">
+      <c r="P273" s="72" t="str">
         <f>IF($N273="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N273,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N273,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="274" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P274" s="69" t="str">
+      <c r="P274" s="72" t="str">
         <f>IF($N274="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N274,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N274,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="275" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P275" s="69" t="str">
+      <c r="P275" s="72" t="str">
         <f>IF($N275="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N275,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N275,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="276" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P276" s="69" t="str">
+      <c r="P276" s="72" t="str">
         <f>IF($N276="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N276,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N276,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="277" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P277" s="69" t="str">
+      <c r="P277" s="72" t="str">
         <f>IF($N277="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N277,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N277,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="278" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P278" s="69" t="str">
+      <c r="P278" s="72" t="str">
         <f>IF($N278="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N278,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N278,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="279" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P279" s="69" t="str">
+      <c r="P279" s="72" t="str">
         <f>IF($N279="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N279,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N279,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="280" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P280" s="69" t="str">
+      <c r="P280" s="72" t="str">
         <f>IF($N280="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N280,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N280,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="281" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P281" s="69" t="str">
+      <c r="P281" s="72" t="str">
         <f>IF($N281="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N281,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N281,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="282" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P282" s="69" t="str">
+      <c r="P282" s="72" t="str">
         <f>IF($N282="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N282,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N282,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="283" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P283" s="69" t="str">
+      <c r="P283" s="72" t="str">
         <f>IF($N283="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N283,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N283,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="284" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P284" s="69" t="str">
+      <c r="P284" s="72" t="str">
         <f>IF($N284="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N284,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N284,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="285" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P285" s="69" t="str">
+      <c r="P285" s="72" t="str">
         <f>IF($N285="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N285,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N285,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="286" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P286" s="69" t="str">
+      <c r="P286" s="72" t="str">
         <f>IF($N286="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N286,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N286,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="287" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P287" s="69" t="str">
+      <c r="P287" s="72" t="str">
         <f>IF($N287="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N287,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N287,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="288" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P288" s="69" t="str">
+      <c r="P288" s="72" t="str">
         <f>IF($N288="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N288,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N288,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="289" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P289" s="69" t="str">
+      <c r="P289" s="72" t="str">
         <f>IF($N289="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N289,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N289,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="290" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P290" s="69" t="str">
+      <c r="P290" s="72" t="str">
         <f>IF($N290="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N290,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N290,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="291" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P291" s="69" t="str">
+      <c r="P291" s="72" t="str">
         <f>IF($N291="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N291,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N291,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="292" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P292" s="69" t="str">
+      <c r="P292" s="72" t="str">
         <f>IF($N292="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N292,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N292,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="293" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P293" s="69" t="str">
+      <c r="P293" s="72" t="str">
         <f>IF($N293="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N293,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N293,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="294" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P294" s="69" t="str">
+      <c r="P294" s="72" t="str">
         <f>IF($N294="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N294,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N294,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="295" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P295" s="69" t="str">
+      <c r="P295" s="72" t="str">
         <f>IF($N295="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N295,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N295,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="296" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P296" s="69" t="str">
+      <c r="P296" s="72" t="str">
         <f>IF($N296="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N296,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N296,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="297" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P297" s="69" t="str">
+      <c r="P297" s="72" t="str">
         <f>IF($N297="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N297,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N297,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="298" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P298" s="69" t="str">
+      <c r="P298" s="72" t="str">
         <f>IF($N298="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N298,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N298,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="299" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P299" s="69" t="str">
+      <c r="P299" s="72" t="str">
         <f>IF($N299="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N299,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N299,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="300" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P300" s="69" t="str">
+      <c r="P300" s="72" t="str">
         <f>IF($N300="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N300,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N300,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="301" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P301" s="69" t="str">
+      <c r="P301" s="72" t="str">
         <f>IF($N301="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N301,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N301,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="302" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P302" s="69" t="str">
+      <c r="P302" s="72" t="str">
         <f>IF($N302="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N302,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N302,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="303" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P303" s="69" t="str">
+      <c r="P303" s="72" t="str">
         <f>IF($N303="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N303,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N303,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="304" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P304" s="69" t="str">
+      <c r="P304" s="72" t="str">
         <f>IF($N304="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N304,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N304,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="305" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P305" s="69" t="str">
+      <c r="P305" s="72" t="str">
         <f>IF($N305="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N305,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N305,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="306" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P306" s="69" t="str">
+      <c r="P306" s="72" t="str">
         <f>IF($N306="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N306,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N306,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="307" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P307" s="69" t="str">
+      <c r="P307" s="72" t="str">
         <f>IF($N307="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N307,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N307,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="308" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P308" s="69" t="str">
+      <c r="P308" s="72" t="str">
         <f>IF($N308="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N308,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N308,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="309" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P309" s="69" t="str">
+      <c r="P309" s="72" t="str">
         <f>IF($N309="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N309,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N309,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="310" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P310" s="69" t="str">
+      <c r="P310" s="72" t="str">
         <f>IF($N310="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N310,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N310,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="311" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P311" s="69" t="str">
+      <c r="P311" s="72" t="str">
         <f>IF($N311="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N311,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N311,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="312" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P312" s="69" t="str">
+      <c r="P312" s="72" t="str">
         <f>IF($N312="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N312,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N312,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="313" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P313" s="69" t="str">
+      <c r="P313" s="72" t="str">
         <f>IF($N313="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N313,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N313,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="314" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P314" s="69" t="str">
+      <c r="P314" s="72" t="str">
         <f>IF($N314="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N314,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N314,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="315" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P315" s="69" t="str">
+      <c r="P315" s="72" t="str">
         <f>IF($N315="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N315,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N315,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="316" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P316" s="69" t="str">
+      <c r="P316" s="72" t="str">
         <f>IF($N316="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N316,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N316,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="317" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P317" s="69" t="str">
+      <c r="P317" s="72" t="str">
         <f>IF($N317="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N317,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N317,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="318" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P318" s="69" t="str">
+      <c r="P318" s="72" t="str">
         <f>IF($N318="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N318,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N318,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="319" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P319" s="69" t="str">
+      <c r="P319" s="72" t="str">
         <f>IF($N319="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N319,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N319,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="320" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P320" s="69" t="str">
+      <c r="P320" s="72" t="str">
         <f>IF($N320="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N320,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N320,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="321" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P321" s="69" t="str">
+      <c r="P321" s="72" t="str">
         <f>IF($N321="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N321,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N321,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="322" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P322" s="69" t="str">
+      <c r="P322" s="72" t="str">
         <f>IF($N322="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N322,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N322,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="323" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P323" s="69" t="str">
+      <c r="P323" s="72" t="str">
         <f>IF($N323="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N323,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N323,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="324" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P324" s="69" t="str">
+      <c r="P324" s="72" t="str">
         <f>IF($N324="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N324,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N324,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="325" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P325" s="69" t="str">
+      <c r="P325" s="72" t="str">
         <f>IF($N325="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N325,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N325,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="326" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P326" s="69" t="str">
+      <c r="P326" s="72" t="str">
         <f>IF($N326="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N326,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N326,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="327" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P327" s="69" t="str">
+      <c r="P327" s="72" t="str">
         <f>IF($N327="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N327,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N327,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="328" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P328" s="69" t="str">
+      <c r="P328" s="72" t="str">
         <f>IF($N328="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N328,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N328,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="329" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P329" s="69" t="str">
+      <c r="P329" s="72" t="str">
         <f>IF($N329="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N329,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N329,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="330" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P330" s="69" t="str">
+      <c r="P330" s="72" t="str">
         <f>IF($N330="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N330,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N330,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="331" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P331" s="69" t="str">
+      <c r="P331" s="72" t="str">
         <f>IF($N331="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N331,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N331,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="332" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P332" s="69" t="str">
+      <c r="P332" s="72" t="str">
         <f>IF($N332="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N332,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N332,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="333" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P333" s="69" t="str">
+      <c r="P333" s="72" t="str">
         <f>IF($N333="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N333,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N333,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="334" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P334" s="69" t="str">
+      <c r="P334" s="72" t="str">
         <f>IF($N334="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N334,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N334,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="335" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P335" s="69" t="str">
+      <c r="P335" s="72" t="str">
         <f>IF($N335="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N335,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N335,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="336" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P336" s="69" t="str">
+      <c r="P336" s="72" t="str">
         <f>IF($N336="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N336,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N336,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="337" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P337" s="69" t="str">
+      <c r="P337" s="72" t="str">
         <f>IF($N337="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N337,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N337,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="338" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P338" s="69" t="str">
+      <c r="P338" s="72" t="str">
         <f>IF($N338="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N338,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N338,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="339" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P339" s="69" t="str">
+      <c r="P339" s="72" t="str">
         <f>IF($N339="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N339,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N339,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="340" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P340" s="69" t="str">
+      <c r="P340" s="72" t="str">
         <f>IF($N340="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N340,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N340,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="341" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P341" s="69" t="str">
+      <c r="P341" s="72" t="str">
         <f>IF($N341="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N341,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N341,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="342" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P342" s="69" t="str">
+      <c r="P342" s="72" t="str">
         <f>IF($N342="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N342,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N342,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="343" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P343" s="69" t="str">
+      <c r="P343" s="72" t="str">
         <f>IF($N343="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N343,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N343,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="344" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P344" s="69" t="str">
+      <c r="P344" s="72" t="str">
         <f>IF($N344="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N344,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N344,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="345" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P345" s="69" t="str">
+      <c r="P345" s="72" t="str">
         <f>IF($N345="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N345,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N345,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="346" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P346" s="69" t="str">
+      <c r="P346" s="72" t="str">
         <f>IF($N346="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N346,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N346,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="347" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P347" s="69" t="str">
+      <c r="P347" s="72" t="str">
         <f>IF($N347="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N347,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N347,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="348" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P348" s="69" t="str">
+      <c r="P348" s="72" t="str">
         <f>IF($N348="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N348,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N348,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="349" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P349" s="69" t="str">
+      <c r="P349" s="72" t="str">
         <f>IF($N349="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N349,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N349,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="350" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P350" s="69" t="str">
+      <c r="P350" s="72" t="str">
         <f>IF($N350="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N350,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N350,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="351" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P351" s="69" t="str">
+      <c r="P351" s="72" t="str">
         <f>IF($N351="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N351,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N351,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="352" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P352" s="69" t="str">
+      <c r="P352" s="72" t="str">
         <f>IF($N352="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N352,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N352,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="353" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P353" s="69" t="str">
+      <c r="P353" s="72" t="str">
         <f>IF($N353="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N353,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N353,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="354" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P354" s="69" t="str">
+      <c r="P354" s="72" t="str">
         <f>IF($N354="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N354,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N354,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="355" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P355" s="69" t="str">
+      <c r="P355" s="72" t="str">
         <f>IF($N355="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N355,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N355,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="356" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P356" s="69" t="str">
+      <c r="P356" s="72" t="str">
         <f>IF($N356="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N356,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N356,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="357" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P357" s="69" t="str">
+      <c r="P357" s="72" t="str">
         <f>IF($N357="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N357,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N357,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="358" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P358" s="69" t="str">
+      <c r="P358" s="72" t="str">
         <f>IF($N358="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N358,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N358,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="359" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P359" s="69" t="str">
+      <c r="P359" s="72" t="str">
         <f>IF($N359="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N359,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N359,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="360" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P360" s="69" t="str">
+      <c r="P360" s="72" t="str">
         <f>IF($N360="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N360,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N360,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="361" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P361" s="69" t="str">
+      <c r="P361" s="72" t="str">
         <f>IF($N361="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N361,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N361,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="362" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P362" s="69" t="str">
+      <c r="P362" s="72" t="str">
         <f>IF($N362="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N362,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N362,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="363" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P363" s="69" t="str">
+      <c r="P363" s="72" t="str">
         <f>IF($N363="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N363,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N363,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="364" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P364" s="69" t="str">
+      <c r="P364" s="72" t="str">
         <f>IF($N364="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N364,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N364,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="365" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P365" s="69" t="str">
+      <c r="P365" s="72" t="str">
         <f>IF($N365="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N365,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N365,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="366" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P366" s="69" t="str">
+      <c r="P366" s="72" t="str">
         <f>IF($N366="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N366,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N366,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="367" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P367" s="69" t="str">
+      <c r="P367" s="72" t="str">
         <f>IF($N367="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N367,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N367,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="368" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P368" s="69" t="str">
+      <c r="P368" s="72" t="str">
         <f>IF($N368="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N368,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N368,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="369" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P369" s="69" t="str">
+      <c r="P369" s="72" t="str">
         <f>IF($N369="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N369,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N369,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="370" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P370" s="69" t="str">
+      <c r="P370" s="72" t="str">
         <f>IF($N370="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N370,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N370,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="371" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P371" s="69" t="str">
+      <c r="P371" s="72" t="str">
         <f>IF($N371="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N371,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N371,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="372" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P372" s="69" t="str">
+      <c r="P372" s="72" t="str">
         <f>IF($N372="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N372,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N372,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="373" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P373" s="69" t="str">
+      <c r="P373" s="72" t="str">
         <f>IF($N373="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N373,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N373,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="374" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P374" s="69" t="str">
+      <c r="P374" s="72" t="str">
         <f>IF($N374="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N374,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N374,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="375" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P375" s="69" t="str">
+      <c r="P375" s="72" t="str">
         <f>IF($N375="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N375,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N375,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="376" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P376" s="69" t="str">
+      <c r="P376" s="72" t="str">
         <f>IF($N376="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N376,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N376,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="377" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P377" s="69" t="str">
+      <c r="P377" s="72" t="str">
         <f>IF($N377="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N377,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N377,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="378" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P378" s="69" t="str">
+      <c r="P378" s="72" t="str">
         <f>IF($N378="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N378,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N378,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="379" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P379" s="69" t="str">
+      <c r="P379" s="72" t="str">
         <f>IF($N379="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N379,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N379,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="380" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P380" s="69" t="str">
+      <c r="P380" s="72" t="str">
         <f>IF($N380="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N380,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N380,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="381" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P381" s="69" t="str">
+      <c r="P381" s="72" t="str">
         <f>IF($N381="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N381,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N381,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="382" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P382" s="69" t="str">
+      <c r="P382" s="72" t="str">
         <f>IF($N382="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N382,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N382,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="383" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P383" s="69" t="str">
+      <c r="P383" s="72" t="str">
         <f>IF($N383="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N383,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N383,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="384" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P384" s="69" t="str">
+      <c r="P384" s="72" t="str">
         <f>IF($N384="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N384,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N384,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="385" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P385" s="69" t="str">
+      <c r="P385" s="72" t="str">
         <f>IF($N385="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N385,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N385,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="386" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P386" s="69" t="str">
+      <c r="P386" s="72" t="str">
         <f>IF($N386="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N386,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N386,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="387" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P387" s="69" t="str">
+      <c r="P387" s="72" t="str">
         <f>IF($N387="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N387,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N387,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="388" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P388" s="69" t="str">
+      <c r="P388" s="72" t="str">
         <f>IF($N388="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N388,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N388,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="389" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P389" s="69" t="str">
+      <c r="P389" s="72" t="str">
         <f>IF($N389="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N389,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N389,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="390" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P390" s="69" t="str">
+      <c r="P390" s="72" t="str">
         <f>IF($N390="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N390,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N390,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="391" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P391" s="69" t="str">
+      <c r="P391" s="72" t="str">
         <f>IF($N391="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N391,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N391,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="392" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P392" s="69" t="str">
+      <c r="P392" s="72" t="str">
         <f>IF($N392="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N392,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N392,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="393" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P393" s="69" t="str">
+      <c r="P393" s="72" t="str">
         <f>IF($N393="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N393,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N393,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="394" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P394" s="69" t="str">
+      <c r="P394" s="72" t="str">
         <f>IF($N394="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N394,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N394,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="395" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P395" s="69" t="str">
+      <c r="P395" s="72" t="str">
         <f>IF($N395="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N395,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N395,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="396" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P396" s="69" t="str">
+      <c r="P396" s="72" t="str">
         <f>IF($N396="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N396,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N396,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="397" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P397" s="69" t="str">
+      <c r="P397" s="72" t="str">
         <f>IF($N397="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N397,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N397,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="398" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P398" s="69" t="str">
+      <c r="P398" s="72" t="str">
         <f>IF($N398="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N398,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N398,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="399" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P399" s="69" t="str">
+      <c r="P399" s="72" t="str">
         <f>IF($N399="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N399,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N399,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="400" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P400" s="69" t="str">
+      <c r="P400" s="72" t="str">
         <f>IF($N400="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N400,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N400,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="401" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P401" s="69" t="str">
+      <c r="P401" s="72" t="str">
         <f>IF($N401="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N401,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N401,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="402" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P402" s="69" t="str">
+      <c r="P402" s="72" t="str">
         <f>IF($N402="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N402,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N402,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="403" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P403" s="69" t="str">
+      <c r="P403" s="72" t="str">
         <f>IF($N403="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N403,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N403,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="404" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P404" s="69" t="str">
+      <c r="P404" s="72" t="str">
         <f>IF($N404="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N404,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N404,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="405" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P405" s="69" t="str">
+      <c r="P405" s="72" t="str">
         <f>IF($N405="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N405,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N405,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="406" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P406" s="69" t="str">
+      <c r="P406" s="72" t="str">
         <f>IF($N406="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N406,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N406,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="407" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P407" s="69" t="str">
+      <c r="P407" s="72" t="str">
         <f>IF($N407="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N407,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N407,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="408" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P408" s="69" t="str">
+      <c r="P408" s="72" t="str">
         <f>IF($N408="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N408,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N408,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="409" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P409" s="69" t="str">
+      <c r="P409" s="72" t="str">
         <f>IF($N409="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N409,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N409,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="410" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P410" s="69" t="str">
+      <c r="P410" s="72" t="str">
         <f>IF($N410="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N410,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N410,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="411" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P411" s="69" t="str">
+      <c r="P411" s="72" t="str">
         <f>IF($N411="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N411,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N411,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="412" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P412" s="69" t="str">
+      <c r="P412" s="72" t="str">
         <f>IF($N412="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N412,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N412,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="413" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P413" s="69" t="str">
+      <c r="P413" s="72" t="str">
         <f>IF($N413="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N413,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N413,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="414" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P414" s="69" t="str">
+      <c r="P414" s="72" t="str">
         <f>IF($N414="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N414,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N414,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="415" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P415" s="69" t="str">
+      <c r="P415" s="72" t="str">
         <f>IF($N415="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N415,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N415,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="416" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P416" s="69" t="str">
+      <c r="P416" s="72" t="str">
         <f>IF($N416="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N416,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N416,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="417" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P417" s="69" t="str">
+      <c r="P417" s="72" t="str">
         <f>IF($N417="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N417,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N417,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="418" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P418" s="69" t="str">
+      <c r="P418" s="72" t="str">
         <f>IF($N418="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N418,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N418,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="419" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P419" s="69" t="str">
+      <c r="P419" s="72" t="str">
         <f>IF($N419="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N419,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N419,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="420" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P420" s="69" t="str">
+      <c r="P420" s="72" t="str">
         <f>IF($N420="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N420,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N420,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="421" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P421" s="69" t="str">
+      <c r="P421" s="72" t="str">
         <f>IF($N421="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N421,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N421,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="422" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P422" s="69" t="str">
+      <c r="P422" s="72" t="str">
         <f>IF($N422="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N422,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N422,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="423" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P423" s="69" t="str">
+      <c r="P423" s="72" t="str">
         <f>IF($N423="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N423,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N423,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="424" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P424" s="69" t="str">
+      <c r="P424" s="72" t="str">
         <f>IF($N424="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N424,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N424,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="425" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P425" s="69" t="str">
+      <c r="P425" s="72" t="str">
         <f>IF($N425="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N425,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N425,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="426" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P426" s="69" t="str">
+      <c r="P426" s="72" t="str">
         <f>IF($N426="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N426,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N426,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="427" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P427" s="69" t="str">
+      <c r="P427" s="72" t="str">
         <f>IF($N427="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N427,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N427,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="428" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P428" s="69" t="str">
+      <c r="P428" s="72" t="str">
         <f>IF($N428="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N428,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N428,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="429" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P429" s="69" t="str">
+      <c r="P429" s="72" t="str">
         <f>IF($N429="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N429,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N429,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="430" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P430" s="69" t="str">
+      <c r="P430" s="72" t="str">
         <f>IF($N430="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N430,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N430,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="431" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P431" s="69" t="str">
+      <c r="P431" s="72" t="str">
         <f>IF($N431="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N431,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N431,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="432" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P432" s="69" t="str">
+      <c r="P432" s="72" t="str">
         <f>IF($N432="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N432,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N432,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="433" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P433" s="69" t="str">
+      <c r="P433" s="72" t="str">
         <f>IF($N433="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N433,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N433,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="434" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P434" s="69" t="str">
+      <c r="P434" s="72" t="str">
         <f>IF($N434="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N434,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N434,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="435" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P435" s="69" t="str">
+      <c r="P435" s="72" t="str">
         <f>IF($N435="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N435,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N435,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="436" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P436" s="69" t="str">
+      <c r="P436" s="72" t="str">
         <f>IF($N436="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N436,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N436,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="437" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P437" s="69" t="str">
+      <c r="P437" s="72" t="str">
         <f>IF($N437="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N437,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N437,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="438" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P438" s="69" t="str">
+      <c r="P438" s="72" t="str">
         <f>IF($N438="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N438,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N438,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="439" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P439" s="69" t="str">
+      <c r="P439" s="72" t="str">
         <f>IF($N439="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N439,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N439,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="440" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P440" s="69" t="str">
+      <c r="P440" s="72" t="str">
         <f>IF($N440="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N440,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N440,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="441" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P441" s="69" t="str">
+      <c r="P441" s="72" t="str">
         <f>IF($N441="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N441,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N441,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="442" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P442" s="69" t="str">
+      <c r="P442" s="72" t="str">
         <f>IF($N442="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N442,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N442,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="443" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P443" s="69" t="str">
+      <c r="P443" s="72" t="str">
         <f>IF($N443="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N443,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N443,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="444" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P444" s="69" t="str">
+      <c r="P444" s="72" t="str">
         <f>IF($N444="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N444,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N444,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="445" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P445" s="69" t="str">
+      <c r="P445" s="72" t="str">
         <f>IF($N445="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N445,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N445,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="446" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P446" s="69" t="str">
+      <c r="P446" s="72" t="str">
         <f>IF($N446="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N446,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N446,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="447" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P447" s="69" t="str">
+      <c r="P447" s="72" t="str">
         <f>IF($N447="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N447,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N447,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="448" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P448" s="69" t="str">
+      <c r="P448" s="72" t="str">
         <f>IF($N448="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N448,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N448,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="449" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P449" s="69" t="str">
+      <c r="P449" s="72" t="str">
         <f>IF($N449="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N449,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N449,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="450" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P450" s="69" t="str">
+      <c r="P450" s="72" t="str">
         <f>IF($N450="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N450,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N450,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="451" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P451" s="69" t="str">
+      <c r="P451" s="72" t="str">
         <f>IF($N451="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N451,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N451,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="452" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P452" s="69" t="str">
+      <c r="P452" s="72" t="str">
         <f>IF($N452="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N452,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N452,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="453" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P453" s="69" t="str">
+      <c r="P453" s="72" t="str">
         <f>IF($N453="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N453,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N453,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="454" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P454" s="69" t="str">
+      <c r="P454" s="72" t="str">
         <f>IF($N454="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N454,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N454,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="455" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P455" s="69" t="str">
+      <c r="P455" s="72" t="str">
         <f>IF($N455="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N455,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N455,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="456" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P456" s="69" t="str">
+      <c r="P456" s="72" t="str">
         <f>IF($N456="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N456,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N456,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="457" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P457" s="69" t="str">
+      <c r="P457" s="72" t="str">
         <f>IF($N457="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N457,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N457,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="458" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P458" s="69" t="str">
+      <c r="P458" s="72" t="str">
         <f>IF($N458="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N458,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N458,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="459" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P459" s="69" t="str">
+      <c r="P459" s="72" t="str">
         <f>IF($N459="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N459,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N459,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="460" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P460" s="69" t="str">
+      <c r="P460" s="72" t="str">
         <f>IF($N460="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N460,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N460,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="461" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P461" s="69" t="str">
+      <c r="P461" s="72" t="str">
         <f>IF($N461="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N461,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N461,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="462" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P462" s="69" t="str">
+      <c r="P462" s="72" t="str">
         <f>IF($N462="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N462,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N462,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="463" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P463" s="69" t="str">
+      <c r="P463" s="72" t="str">
         <f>IF($N463="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N463,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N463,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="464" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P464" s="69" t="str">
+      <c r="P464" s="72" t="str">
         <f>IF($N464="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N464,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N464,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="465" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P465" s="69" t="str">
+      <c r="P465" s="72" t="str">
         <f>IF($N465="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N465,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N465,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="466" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P466" s="69" t="str">
+      <c r="P466" s="72" t="str">
         <f>IF($N466="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N466,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N466,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="467" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P467" s="69" t="str">
+      <c r="P467" s="72" t="str">
         <f>IF($N467="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N467,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N467,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="468" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P468" s="69" t="str">
+      <c r="P468" s="72" t="str">
         <f>IF($N468="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N468,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N468,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="469" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P469" s="69" t="str">
+      <c r="P469" s="72" t="str">
         <f>IF($N469="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N469,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N469,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="470" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P470" s="69" t="str">
+      <c r="P470" s="72" t="str">
         <f>IF($N470="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N470,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N470,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="471" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P471" s="69" t="str">
+      <c r="P471" s="72" t="str">
         <f>IF($N471="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N471,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N471,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="472" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P472" s="69" t="str">
+      <c r="P472" s="72" t="str">
         <f>IF($N472="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N472,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N472,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="473" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P473" s="69" t="str">
+      <c r="P473" s="72" t="str">
         <f>IF($N473="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N473,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N473,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="474" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P474" s="69" t="str">
+      <c r="P474" s="72" t="str">
         <f>IF($N474="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N474,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N474,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="475" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P475" s="69" t="str">
+      <c r="P475" s="72" t="str">
         <f>IF($N475="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N475,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N475,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="476" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P476" s="69" t="str">
+      <c r="P476" s="72" t="str">
         <f>IF($N476="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N476,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N476,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="477" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P477" s="69" t="str">
+      <c r="P477" s="72" t="str">
         <f>IF($N477="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N477,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N477,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="478" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P478" s="69" t="str">
+      <c r="P478" s="72" t="str">
         <f>IF($N478="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N478,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N478,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="479" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P479" s="69" t="str">
+      <c r="P479" s="72" t="str">
         <f>IF($N479="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N479,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N479,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="480" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P480" s="69" t="str">
+      <c r="P480" s="72" t="str">
         <f>IF($N480="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N480,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N480,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="481" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P481" s="69" t="str">
+      <c r="P481" s="72" t="str">
         <f>IF($N481="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N481,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N481,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="482" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P482" s="69" t="str">
+      <c r="P482" s="72" t="str">
         <f>IF($N482="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N482,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N482,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="483" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P483" s="69" t="str">
+      <c r="P483" s="72" t="str">
         <f>IF($N483="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N483,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N483,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="484" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P484" s="69" t="str">
+      <c r="P484" s="72" t="str">
         <f>IF($N484="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N484,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N484,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="485" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P485" s="69" t="str">
+      <c r="P485" s="72" t="str">
         <f>IF($N485="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N485,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N485,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="486" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P486" s="69" t="str">
+      <c r="P486" s="72" t="str">
         <f>IF($N486="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N486,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N486,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="487" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P487" s="69" t="str">
+      <c r="P487" s="72" t="str">
         <f>IF($N487="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N487,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N487,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="488" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P488" s="69" t="str">
+      <c r="P488" s="72" t="str">
         <f>IF($N488="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N488,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N488,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="489" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P489" s="69" t="str">
+      <c r="P489" s="72" t="str">
         <f>IF($N489="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N489,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N489,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="490" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P490" s="69" t="str">
+      <c r="P490" s="72" t="str">
         <f>IF($N490="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N490,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N490,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="491" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P491" s="69" t="str">
+      <c r="P491" s="72" t="str">
         <f>IF($N491="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N491,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N491,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="492" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P492" s="69" t="str">
+      <c r="P492" s="72" t="str">
         <f>IF($N492="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N492,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N492,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="493" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P493" s="69" t="str">
+      <c r="P493" s="72" t="str">
         <f>IF($N493="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N493,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N493,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="494" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P494" s="69" t="str">
+      <c r="P494" s="72" t="str">
         <f>IF($N494="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N494,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N494,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="495" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P495" s="69" t="str">
+      <c r="P495" s="72" t="str">
         <f>IF($N495="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N495,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N495,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="496" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P496" s="69" t="str">
+      <c r="P496" s="72" t="str">
         <f>IF($N496="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N496,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N496,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="497" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P497" s="69" t="str">
+      <c r="P497" s="72" t="str">
         <f>IF($N497="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N497,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N497,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="498" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P498" s="69" t="str">
+      <c r="P498" s="72" t="str">
         <f>IF($N498="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N498,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N498,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="499" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P499" s="69" t="str">
+      <c r="P499" s="72" t="str">
         <f>IF($N499="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N499,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N499,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="500" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P500" s="69" t="str">
+      <c r="P500" s="72" t="str">
         <f>IF($N500="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N500,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N500,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="501" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P501" s="69" t="str">
+      <c r="P501" s="72" t="str">
         <f>IF($N501="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N501,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N501,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="502" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P502" s="69" t="str">
+      <c r="P502" s="72" t="str">
         <f>IF($N502="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N502,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N502,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
     </row>
     <row r="503" spans="16:16" x14ac:dyDescent="0.15">
-      <c r="P503" s="69" t="str">
+      <c r="P503" s="72" t="str">
         <f>IF($N503="","",IF(OR(RawResults!$E$8="No",RawResults!$K$8="No"),"N/A",IF(VLOOKUP($N503,RawResults!$B$13:$P$513,12,FALSE)=0,"",VLOOKUP($N503,RawResults!$B$13:$P$513,12,FALSE))))</f>
         <v/>
       </c>
@@ -5337,18 +5303,18 @@
   </sheetPr>
   <dimension ref="A1:P513"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="12" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.6640625" style="7" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="28" style="73" customWidth="1"/>
+    <col min="3" max="3" width="28" style="69" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="7.5" style="19" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" style="19" customWidth="1"/>
@@ -5367,48 +5333,48 @@
   <sheetData>
     <row r="1" spans="1:16" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="71"/>
+      <c r="D1" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="55" t="s">
+      <c r="G1" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="H1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="I1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="J1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="K1" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="L1" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="M1" s="53" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="53" t="s">
-        <v>27</v>
       </c>
       <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:16" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="68"/>
+      <c r="D2" s="51" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="51" t="s">
-        <v>30</v>
       </c>
       <c r="E2" s="56"/>
       <c r="F2" s="49"/>
@@ -5432,11 +5398,11 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="72"/>
+        <v>29</v>
+      </c>
+      <c r="C3" s="68"/>
       <c r="D3" s="52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="57">
         <f>COUNTIF(RawResults!$M$13:$M$499,"&gt; ")-SUM(F3:$L$3)</f>
@@ -5479,9 +5445,9 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="72"/>
+        <v>11</v>
+      </c>
+      <c r="C4" s="68"/>
       <c r="D4" s="52"/>
       <c r="E4" s="60">
         <f>IF($M$3=0,0,E3/$M$3)</f>
@@ -5524,9 +5490,9 @@
     </row>
     <row r="5" spans="1:16" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="72"/>
+        <v>31</v>
+      </c>
+      <c r="C5" s="68"/>
       <c r="D5" s="63"/>
       <c r="E5" s="64" t="str">
         <f>IF($M$3=0,"",IF(E3/$M$3&gt;0.5,"Query","OK"))</f>
@@ -5567,10 +5533,10 @@
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -5585,20 +5551,20 @@
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="40" t="s">
         <v>35</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>37</v>
       </c>
       <c r="F7" s="35"/>
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
       <c r="I7" s="45"/>
       <c r="K7" s="38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L7" s="39"/>
       <c r="M7" s="34"/>
@@ -5607,14 +5573,14 @@
       <c r="P7" s="22"/>
     </row>
     <row r="8" spans="1:16" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="E8" s="71" t="s">
-        <v>39</v>
+      <c r="E8" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
       <c r="H8" s="21"/>
-      <c r="K8" s="71" t="s">
-        <v>39</v>
+      <c r="K8" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
@@ -5638,7 +5604,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B10" s="7"/>
       <c r="D10" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="31">
         <v>0</v>
@@ -5670,9 +5636,9 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B11" s="9"/>
-      <c r="C11" s="74"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="32">
         <v>1</v>
@@ -5700,13 +5666,13 @@
     </row>
     <row r="12" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="B12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="D12" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="33"/>
@@ -5715,22 +5681,22 @@
       <c r="I12" s="33"/>
       <c r="J12" s="33"/>
       <c r="K12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="43" t="s">
+      <c r="N12" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="M12" s="43" t="s">
+      <c r="O12" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="P12" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="O12" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -19321,187 +19287,187 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.15">
       <c r="D5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.15">
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle more options for text+value results, variable student ID location and overall grade column
</commit_message>
<xml_diff>
--- a/data/subject_results/Blank-Results.xlsx
+++ b/data/subject_results/Blank-Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sci-lmw1/dev/HelpLindsay/data/subject_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBD39BC-EAEC-4344-99F3-C20123EE16FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B0026-DF0E-1A48-AA39-C85569B892B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="519" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5060" windowWidth="28800" windowHeight="17540" tabRatio="519" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StudentOne" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
   <si>
     <t xml:space="preserve">FORMAT STUDY_PACKAGE_RESULT STANDARD </t>
   </si>
@@ -165,9 +165,6 @@
     <t>Final Grade</t>
   </si>
   <si>
-    <t>ED/NS</t>
-  </si>
-  <si>
     <t>Override EM</t>
   </si>
   <si>
@@ -253,6 +250,27 @@
   </si>
   <si>
     <t>Parent Ssp No</t>
+  </si>
+  <si>
+    <t>Valid other grades</t>
+  </si>
+  <si>
+    <t>Result Withheld (student assessment requirements are outstanding)</t>
+  </si>
+  <si>
+    <t>Assessment Incomplete (College assessment process is incomplete)</t>
+  </si>
+  <si>
+    <t>Fail (supplementary examination granted)</t>
+  </si>
+  <si>
+    <t>Fail (supplementary assessment granted)</t>
+  </si>
+  <si>
+    <t>Deferred examination granted</t>
+  </si>
+  <si>
+    <t>Interim result for a subject which forms part of a subject chain</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1104,7 @@
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -1281,6 +1299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1329,7 +1348,27 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1355,8 +1394,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2180,9 +2219,9 @@
   </sheetPr>
   <dimension ref="A1:Q503"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2215,7 +2254,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="72" t="s">
         <v>1</v>
@@ -5301,13 +5340,13 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:P513"/>
+  <dimension ref="A1:R513"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="12" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C2:C5"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5331,7 +5370,7 @@
     <col min="25" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5367,8 +5406,11 @@
         <v>25</v>
       </c>
       <c r="O1" s="21"/>
-    </row>
-    <row r="2" spans="1:16" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q1" s="75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
@@ -5395,8 +5437,14 @@
       <c r="M2" s="54"/>
       <c r="O2" s="26"/>
       <c r="P2" s="26"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -5442,8 +5490,14 @@
       </c>
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="Q3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
@@ -5487,8 +5541,14 @@
       </c>
       <c r="O4" s="26"/>
       <c r="P4" s="26"/>
-    </row>
-    <row r="5" spans="1:16" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="Q4" t="s">
+        <v>62</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
@@ -5530,8 +5590,14 @@
       <c r="N5" s="27"/>
       <c r="O5" s="27"/>
       <c r="P5" s="28"/>
-    </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="Q5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -5548,8 +5614,14 @@
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
-    </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
@@ -5571,8 +5643,14 @@
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
       <c r="P7" s="22"/>
-    </row>
-    <row r="8" spans="1:16" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="Q7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="E8" s="67" t="s">
         <v>37</v>
       </c>
@@ -5588,7 +5666,7 @@
       <c r="O8" s="21"/>
       <c r="P8" s="22"/>
     </row>
-    <row r="9" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -5601,7 +5679,7 @@
       <c r="O9" s="21"/>
       <c r="P9" s="22"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B10" s="7"/>
       <c r="D10" s="6" t="s">
         <v>38</v>
@@ -5634,7 +5712,7 @@
       <c r="O10" s="8"/>
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B11" s="9"/>
       <c r="C11" s="70"/>
       <c r="D11" s="2" t="s">
@@ -5664,7 +5742,7 @@
       <c r="O11" s="7"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" ht="42" x14ac:dyDescent="0.15">
       <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
@@ -5690,16 +5768,16 @@
         <v>43</v>
       </c>
       <c r="N12" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="O12" s="30" t="s">
+      <c r="P12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P12" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="18"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -5719,14 +5797,14 @@
         <v/>
       </c>
       <c r="M13" s="44" t="str">
-        <f t="shared" ref="M13:M27" si="4">IF(OR($C$6="",$C$7=""),"",IF(O13&lt;&gt;"",O13,IF(N13="ED",N13,IF(N13="NS",N13,L13))))</f>
+        <f>IF(OR($C$6="",$C$7=""),"",IF(O13&lt;&gt;"",O13,IF(ISNUMBER(MATCH(N13,Q$2:Q$8,0)),N13,L13)))</f>
         <v/>
       </c>
       <c r="N13" s="37"/>
       <c r="O13" s="42"/>
       <c r="P13" s="14"/>
     </row>
-    <row r="14" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -5746,14 +5824,14 @@
         <v/>
       </c>
       <c r="M14" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="M14:M77" si="4">IF(OR($C$6="",$C$7=""),"",IF(O14&lt;&gt;"",O14,IF(ISNUMBER(MATCH(N14,Q$2:Q$8,0)),N14,L14)))</f>
         <v/>
       </c>
       <c r="N14" s="37"/>
       <c r="O14" s="42"/>
       <c r="P14" s="14"/>
     </row>
-    <row r="15" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="18"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -5780,7 +5858,7 @@
       <c r="O15" s="42"/>
       <c r="P15" s="14"/>
     </row>
-    <row r="16" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="18"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
@@ -6124,7 +6202,7 @@
         <v/>
       </c>
       <c r="M28" s="44" t="str">
-        <f t="shared" ref="M28:M91" si="7">IF(OR($C$6="",$C$7=""),"",IF(O28&lt;&gt;"",O28,IF(N28="ED",N28,IF(N28="NS",N28,L28))))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N28" s="37"/>
@@ -6151,7 +6229,7 @@
         <v/>
       </c>
       <c r="M29" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N29" s="37"/>
@@ -6178,7 +6256,7 @@
         <v/>
       </c>
       <c r="M30" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N30" s="37"/>
@@ -6205,7 +6283,7 @@
         <v/>
       </c>
       <c r="M31" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N31" s="37"/>
@@ -6232,7 +6310,7 @@
         <v/>
       </c>
       <c r="M32" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N32" s="37"/>
@@ -6259,7 +6337,7 @@
         <v/>
       </c>
       <c r="M33" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N33" s="37"/>
@@ -6286,7 +6364,7 @@
         <v/>
       </c>
       <c r="M34" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N34" s="37"/>
@@ -6313,7 +6391,7 @@
         <v/>
       </c>
       <c r="M35" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N35" s="37"/>
@@ -6340,7 +6418,7 @@
         <v/>
       </c>
       <c r="M36" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N36" s="37"/>
@@ -6367,7 +6445,7 @@
         <v/>
       </c>
       <c r="M37" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N37" s="37"/>
@@ -6394,7 +6472,7 @@
         <v/>
       </c>
       <c r="M38" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N38" s="37"/>
@@ -6421,7 +6499,7 @@
         <v/>
       </c>
       <c r="M39" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N39" s="37"/>
@@ -6448,7 +6526,7 @@
         <v/>
       </c>
       <c r="M40" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N40" s="37"/>
@@ -6475,7 +6553,7 @@
         <v/>
       </c>
       <c r="M41" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N41" s="37"/>
@@ -6502,7 +6580,7 @@
         <v/>
       </c>
       <c r="M42" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N42" s="37"/>
@@ -6529,7 +6607,7 @@
         <v/>
       </c>
       <c r="M43" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N43" s="37"/>
@@ -6556,7 +6634,7 @@
         <v/>
       </c>
       <c r="M44" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N44" s="37"/>
@@ -6583,7 +6661,7 @@
         <v/>
       </c>
       <c r="M45" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N45" s="37"/>
@@ -6610,7 +6688,7 @@
         <v/>
       </c>
       <c r="M46" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N46" s="37"/>
@@ -6637,7 +6715,7 @@
         <v/>
       </c>
       <c r="M47" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N47" s="37"/>
@@ -6664,7 +6742,7 @@
         <v/>
       </c>
       <c r="M48" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N48" s="37"/>
@@ -6691,7 +6769,7 @@
         <v/>
       </c>
       <c r="M49" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N49" s="37"/>
@@ -6718,7 +6796,7 @@
         <v/>
       </c>
       <c r="M50" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N50" s="37"/>
@@ -6745,7 +6823,7 @@
         <v/>
       </c>
       <c r="M51" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N51" s="37"/>
@@ -6772,7 +6850,7 @@
         <v/>
       </c>
       <c r="M52" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N52" s="37"/>
@@ -6799,7 +6877,7 @@
         <v/>
       </c>
       <c r="M53" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N53" s="37"/>
@@ -6826,7 +6904,7 @@
         <v/>
       </c>
       <c r="M54" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N54" s="37"/>
@@ -6853,7 +6931,7 @@
         <v/>
       </c>
       <c r="M55" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N55" s="37"/>
@@ -6880,7 +6958,7 @@
         <v/>
       </c>
       <c r="M56" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N56" s="37"/>
@@ -6907,7 +6985,7 @@
         <v/>
       </c>
       <c r="M57" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N57" s="37"/>
@@ -6934,7 +7012,7 @@
         <v/>
       </c>
       <c r="M58" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N58" s="37"/>
@@ -6961,7 +7039,7 @@
         <v/>
       </c>
       <c r="M59" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N59" s="37"/>
@@ -6988,7 +7066,7 @@
         <v/>
       </c>
       <c r="M60" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N60" s="37"/>
@@ -7015,7 +7093,7 @@
         <v/>
       </c>
       <c r="M61" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N61" s="37"/>
@@ -7042,7 +7120,7 @@
         <v/>
       </c>
       <c r="M62" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N62" s="37"/>
@@ -7069,7 +7147,7 @@
         <v/>
       </c>
       <c r="M63" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N63" s="37"/>
@@ -7096,7 +7174,7 @@
         <v/>
       </c>
       <c r="M64" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N64" s="37"/>
@@ -7123,7 +7201,7 @@
         <v/>
       </c>
       <c r="M65" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N65" s="37"/>
@@ -7150,7 +7228,7 @@
         <v/>
       </c>
       <c r="M66" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N66" s="37"/>
@@ -7177,7 +7255,7 @@
         <v/>
       </c>
       <c r="M67" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N67" s="37"/>
@@ -7204,7 +7282,7 @@
         <v/>
       </c>
       <c r="M68" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N68" s="37"/>
@@ -7231,7 +7309,7 @@
         <v/>
       </c>
       <c r="M69" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N69" s="37"/>
@@ -7258,7 +7336,7 @@
         <v/>
       </c>
       <c r="M70" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N70" s="37"/>
@@ -7285,7 +7363,7 @@
         <v/>
       </c>
       <c r="M71" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N71" s="37"/>
@@ -7312,7 +7390,7 @@
         <v/>
       </c>
       <c r="M72" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N72" s="37"/>
@@ -7339,7 +7417,7 @@
         <v/>
       </c>
       <c r="M73" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N73" s="37"/>
@@ -7366,7 +7444,7 @@
         <v/>
       </c>
       <c r="M74" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N74" s="37"/>
@@ -7393,7 +7471,7 @@
         <v/>
       </c>
       <c r="M75" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N75" s="37"/>
@@ -7420,7 +7498,7 @@
         <v/>
       </c>
       <c r="M76" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N76" s="37"/>
@@ -7447,7 +7525,7 @@
         <v/>
       </c>
       <c r="M77" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N77" s="37"/>
@@ -7474,7 +7552,7 @@
         <v/>
       </c>
       <c r="M78" s="44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="M78:M141" si="7">IF(OR($C$6="",$C$7=""),"",IF(O78&lt;&gt;"",O78,IF(ISNUMBER(MATCH(N78,Q$2:Q$8,0)),N78,L78)))</f>
         <v/>
       </c>
       <c r="N78" s="37"/>
@@ -7852,7 +7930,7 @@
         <v/>
       </c>
       <c r="M92" s="44" t="str">
-        <f t="shared" ref="M92:M155" si="10">IF(OR($C$6="",$C$7=""),"",IF(O92&lt;&gt;"",O92,IF(N92="ED",N92,IF(N92="NS",N92,L92))))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N92" s="37"/>
@@ -7879,7 +7957,7 @@
         <v/>
       </c>
       <c r="M93" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N93" s="37"/>
@@ -7906,7 +7984,7 @@
         <v/>
       </c>
       <c r="M94" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N94" s="37"/>
@@ -7933,7 +8011,7 @@
         <v/>
       </c>
       <c r="M95" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N95" s="37"/>
@@ -7960,7 +8038,7 @@
         <v/>
       </c>
       <c r="M96" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N96" s="37"/>
@@ -7987,7 +8065,7 @@
         <v/>
       </c>
       <c r="M97" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N97" s="37"/>
@@ -8014,7 +8092,7 @@
         <v/>
       </c>
       <c r="M98" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N98" s="37"/>
@@ -8041,7 +8119,7 @@
         <v/>
       </c>
       <c r="M99" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N99" s="37"/>
@@ -8068,7 +8146,7 @@
         <v/>
       </c>
       <c r="M100" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N100" s="37"/>
@@ -8095,7 +8173,7 @@
         <v/>
       </c>
       <c r="M101" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N101" s="37"/>
@@ -8122,7 +8200,7 @@
         <v/>
       </c>
       <c r="M102" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N102" s="37"/>
@@ -8149,7 +8227,7 @@
         <v/>
       </c>
       <c r="M103" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N103" s="37"/>
@@ -8176,7 +8254,7 @@
         <v/>
       </c>
       <c r="M104" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N104" s="37"/>
@@ -8203,7 +8281,7 @@
         <v/>
       </c>
       <c r="M105" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N105" s="37"/>
@@ -8230,7 +8308,7 @@
         <v/>
       </c>
       <c r="M106" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N106" s="37"/>
@@ -8257,7 +8335,7 @@
         <v/>
       </c>
       <c r="M107" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N107" s="37"/>
@@ -8284,7 +8362,7 @@
         <v/>
       </c>
       <c r="M108" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N108" s="37"/>
@@ -8311,7 +8389,7 @@
         <v/>
       </c>
       <c r="M109" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N109" s="37"/>
@@ -8338,7 +8416,7 @@
         <v/>
       </c>
       <c r="M110" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N110" s="37"/>
@@ -8365,7 +8443,7 @@
         <v/>
       </c>
       <c r="M111" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N111" s="37"/>
@@ -8392,7 +8470,7 @@
         <v/>
       </c>
       <c r="M112" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N112" s="37"/>
@@ -8419,7 +8497,7 @@
         <v/>
       </c>
       <c r="M113" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N113" s="37"/>
@@ -8446,7 +8524,7 @@
         <v/>
       </c>
       <c r="M114" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N114" s="37"/>
@@ -8473,7 +8551,7 @@
         <v/>
       </c>
       <c r="M115" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N115" s="37"/>
@@ -8500,7 +8578,7 @@
         <v/>
       </c>
       <c r="M116" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N116" s="37"/>
@@ -8527,7 +8605,7 @@
         <v/>
       </c>
       <c r="M117" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N117" s="37"/>
@@ -8554,7 +8632,7 @@
         <v/>
       </c>
       <c r="M118" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N118" s="37"/>
@@ -8581,7 +8659,7 @@
         <v/>
       </c>
       <c r="M119" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N119" s="37"/>
@@ -8608,7 +8686,7 @@
         <v/>
       </c>
       <c r="M120" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N120" s="37"/>
@@ -8635,7 +8713,7 @@
         <v/>
       </c>
       <c r="M121" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N121" s="37"/>
@@ -8662,7 +8740,7 @@
         <v/>
       </c>
       <c r="M122" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N122" s="37"/>
@@ -8689,7 +8767,7 @@
         <v/>
       </c>
       <c r="M123" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N123" s="37"/>
@@ -8716,7 +8794,7 @@
         <v/>
       </c>
       <c r="M124" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N124" s="37"/>
@@ -8743,7 +8821,7 @@
         <v/>
       </c>
       <c r="M125" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N125" s="37"/>
@@ -8770,7 +8848,7 @@
         <v/>
       </c>
       <c r="M126" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N126" s="37"/>
@@ -8797,7 +8875,7 @@
         <v/>
       </c>
       <c r="M127" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N127" s="37"/>
@@ -8824,7 +8902,7 @@
         <v/>
       </c>
       <c r="M128" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N128" s="37"/>
@@ -8851,7 +8929,7 @@
         <v/>
       </c>
       <c r="M129" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N129" s="37"/>
@@ -8878,7 +8956,7 @@
         <v/>
       </c>
       <c r="M130" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N130" s="37"/>
@@ -8905,7 +8983,7 @@
         <v/>
       </c>
       <c r="M131" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N131" s="37"/>
@@ -8932,7 +9010,7 @@
         <v/>
       </c>
       <c r="M132" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N132" s="37"/>
@@ -8959,7 +9037,7 @@
         <v/>
       </c>
       <c r="M133" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N133" s="37"/>
@@ -8986,7 +9064,7 @@
         <v/>
       </c>
       <c r="M134" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N134" s="37"/>
@@ -9013,7 +9091,7 @@
         <v/>
       </c>
       <c r="M135" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N135" s="37"/>
@@ -9040,7 +9118,7 @@
         <v/>
       </c>
       <c r="M136" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N136" s="37"/>
@@ -9067,7 +9145,7 @@
         <v/>
       </c>
       <c r="M137" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N137" s="37"/>
@@ -9094,7 +9172,7 @@
         <v/>
       </c>
       <c r="M138" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N138" s="37"/>
@@ -9121,7 +9199,7 @@
         <v/>
       </c>
       <c r="M139" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N139" s="37"/>
@@ -9148,7 +9226,7 @@
         <v/>
       </c>
       <c r="M140" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N140" s="37"/>
@@ -9175,7 +9253,7 @@
         <v/>
       </c>
       <c r="M141" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N141" s="37"/>
@@ -9202,7 +9280,7 @@
         <v/>
       </c>
       <c r="M142" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="M142:M205" si="10">IF(OR($C$6="",$C$7=""),"",IF(O142&lt;&gt;"",O142,IF(ISNUMBER(MATCH(N142,Q$2:Q$8,0)),N142,L142)))</f>
         <v/>
       </c>
       <c r="N142" s="37"/>
@@ -9580,7 +9658,7 @@
         <v/>
       </c>
       <c r="M156" s="44" t="str">
-        <f t="shared" ref="M156:M219" si="13">IF(OR($C$6="",$C$7=""),"",IF(O156&lt;&gt;"",O156,IF(N156="ED",N156,IF(N156="NS",N156,L156))))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N156" s="37"/>
@@ -9607,7 +9685,7 @@
         <v/>
       </c>
       <c r="M157" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N157" s="37"/>
@@ -9634,7 +9712,7 @@
         <v/>
       </c>
       <c r="M158" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N158" s="37"/>
@@ -9661,7 +9739,7 @@
         <v/>
       </c>
       <c r="M159" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N159" s="37"/>
@@ -9688,7 +9766,7 @@
         <v/>
       </c>
       <c r="M160" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N160" s="37"/>
@@ -9715,7 +9793,7 @@
         <v/>
       </c>
       <c r="M161" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N161" s="37"/>
@@ -9742,7 +9820,7 @@
         <v/>
       </c>
       <c r="M162" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N162" s="37"/>
@@ -9769,7 +9847,7 @@
         <v/>
       </c>
       <c r="M163" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N163" s="37"/>
@@ -9796,7 +9874,7 @@
         <v/>
       </c>
       <c r="M164" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N164" s="37"/>
@@ -9823,7 +9901,7 @@
         <v/>
       </c>
       <c r="M165" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N165" s="37"/>
@@ -9850,7 +9928,7 @@
         <v/>
       </c>
       <c r="M166" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N166" s="37"/>
@@ -9877,7 +9955,7 @@
         <v/>
       </c>
       <c r="M167" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N167" s="37"/>
@@ -9904,7 +9982,7 @@
         <v/>
       </c>
       <c r="M168" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N168" s="37"/>
@@ -9931,7 +10009,7 @@
         <v/>
       </c>
       <c r="M169" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N169" s="37"/>
@@ -9958,7 +10036,7 @@
         <v/>
       </c>
       <c r="M170" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N170" s="37"/>
@@ -9985,7 +10063,7 @@
         <v/>
       </c>
       <c r="M171" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N171" s="37"/>
@@ -10012,7 +10090,7 @@
         <v/>
       </c>
       <c r="M172" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N172" s="37"/>
@@ -10039,7 +10117,7 @@
         <v/>
       </c>
       <c r="M173" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N173" s="37"/>
@@ -10066,7 +10144,7 @@
         <v/>
       </c>
       <c r="M174" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N174" s="37"/>
@@ -10093,7 +10171,7 @@
         <v/>
       </c>
       <c r="M175" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N175" s="37"/>
@@ -10120,7 +10198,7 @@
         <v/>
       </c>
       <c r="M176" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N176" s="37"/>
@@ -10147,7 +10225,7 @@
         <v/>
       </c>
       <c r="M177" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N177" s="37"/>
@@ -10174,7 +10252,7 @@
         <v/>
       </c>
       <c r="M178" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N178" s="37"/>
@@ -10201,7 +10279,7 @@
         <v/>
       </c>
       <c r="M179" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N179" s="37"/>
@@ -10228,7 +10306,7 @@
         <v/>
       </c>
       <c r="M180" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N180" s="37"/>
@@ -10255,7 +10333,7 @@
         <v/>
       </c>
       <c r="M181" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N181" s="37"/>
@@ -10282,7 +10360,7 @@
         <v/>
       </c>
       <c r="M182" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N182" s="37"/>
@@ -10309,7 +10387,7 @@
         <v/>
       </c>
       <c r="M183" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N183" s="37"/>
@@ -10336,7 +10414,7 @@
         <v/>
       </c>
       <c r="M184" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N184" s="37"/>
@@ -10363,7 +10441,7 @@
         <v/>
       </c>
       <c r="M185" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N185" s="37"/>
@@ -10390,7 +10468,7 @@
         <v/>
       </c>
       <c r="M186" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N186" s="37"/>
@@ -10417,7 +10495,7 @@
         <v/>
       </c>
       <c r="M187" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N187" s="37"/>
@@ -10444,7 +10522,7 @@
         <v/>
       </c>
       <c r="M188" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N188" s="37"/>
@@ -10471,7 +10549,7 @@
         <v/>
       </c>
       <c r="M189" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N189" s="37"/>
@@ -10498,7 +10576,7 @@
         <v/>
       </c>
       <c r="M190" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N190" s="37"/>
@@ -10525,7 +10603,7 @@
         <v/>
       </c>
       <c r="M191" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N191" s="37"/>
@@ -10552,7 +10630,7 @@
         <v/>
       </c>
       <c r="M192" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N192" s="37"/>
@@ -10579,7 +10657,7 @@
         <v/>
       </c>
       <c r="M193" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N193" s="37"/>
@@ -10606,7 +10684,7 @@
         <v/>
       </c>
       <c r="M194" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N194" s="37"/>
@@ -10633,7 +10711,7 @@
         <v/>
       </c>
       <c r="M195" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N195" s="37"/>
@@ -10660,7 +10738,7 @@
         <v/>
       </c>
       <c r="M196" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N196" s="37"/>
@@ -10687,7 +10765,7 @@
         <v/>
       </c>
       <c r="M197" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N197" s="37"/>
@@ -10714,7 +10792,7 @@
         <v/>
       </c>
       <c r="M198" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N198" s="37"/>
@@ -10741,7 +10819,7 @@
         <v/>
       </c>
       <c r="M199" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N199" s="37"/>
@@ -10768,7 +10846,7 @@
         <v/>
       </c>
       <c r="M200" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N200" s="37"/>
@@ -10795,7 +10873,7 @@
         <v/>
       </c>
       <c r="M201" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N201" s="37"/>
@@ -10822,7 +10900,7 @@
         <v/>
       </c>
       <c r="M202" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N202" s="37"/>
@@ -10849,7 +10927,7 @@
         <v/>
       </c>
       <c r="M203" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N203" s="37"/>
@@ -10876,7 +10954,7 @@
         <v/>
       </c>
       <c r="M204" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N204" s="37"/>
@@ -10903,7 +10981,7 @@
         <v/>
       </c>
       <c r="M205" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N205" s="37"/>
@@ -10930,7 +11008,7 @@
         <v/>
       </c>
       <c r="M206" s="44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="M206:M269" si="13">IF(OR($C$6="",$C$7=""),"",IF(O206&lt;&gt;"",O206,IF(ISNUMBER(MATCH(N206,Q$2:Q$8,0)),N206,L206)))</f>
         <v/>
       </c>
       <c r="N206" s="37"/>
@@ -11308,7 +11386,7 @@
         <v/>
       </c>
       <c r="M220" s="44" t="str">
-        <f t="shared" ref="M220:M283" si="16">IF(OR($C$6="",$C$7=""),"",IF(O220&lt;&gt;"",O220,IF(N220="ED",N220,IF(N220="NS",N220,L220))))</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N220" s="37"/>
@@ -11335,7 +11413,7 @@
         <v/>
       </c>
       <c r="M221" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N221" s="37"/>
@@ -11362,7 +11440,7 @@
         <v/>
       </c>
       <c r="M222" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N222" s="37"/>
@@ -11389,7 +11467,7 @@
         <v/>
       </c>
       <c r="M223" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N223" s="37"/>
@@ -11416,7 +11494,7 @@
         <v/>
       </c>
       <c r="M224" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N224" s="37"/>
@@ -11443,7 +11521,7 @@
         <v/>
       </c>
       <c r="M225" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N225" s="37"/>
@@ -11470,7 +11548,7 @@
         <v/>
       </c>
       <c r="M226" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N226" s="37"/>
@@ -11497,7 +11575,7 @@
         <v/>
       </c>
       <c r="M227" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N227" s="37"/>
@@ -11524,7 +11602,7 @@
         <v/>
       </c>
       <c r="M228" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N228" s="37"/>
@@ -11551,7 +11629,7 @@
         <v/>
       </c>
       <c r="M229" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N229" s="37"/>
@@ -11578,7 +11656,7 @@
         <v/>
       </c>
       <c r="M230" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N230" s="37"/>
@@ -11605,7 +11683,7 @@
         <v/>
       </c>
       <c r="M231" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N231" s="37"/>
@@ -11632,7 +11710,7 @@
         <v/>
       </c>
       <c r="M232" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N232" s="37"/>
@@ -11659,7 +11737,7 @@
         <v/>
       </c>
       <c r="M233" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N233" s="37"/>
@@ -11686,7 +11764,7 @@
         <v/>
       </c>
       <c r="M234" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N234" s="37"/>
@@ -11713,7 +11791,7 @@
         <v/>
       </c>
       <c r="M235" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N235" s="37"/>
@@ -11740,7 +11818,7 @@
         <v/>
       </c>
       <c r="M236" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N236" s="37"/>
@@ -11767,7 +11845,7 @@
         <v/>
       </c>
       <c r="M237" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N237" s="37"/>
@@ -11794,7 +11872,7 @@
         <v/>
       </c>
       <c r="M238" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N238" s="37"/>
@@ -11821,7 +11899,7 @@
         <v/>
       </c>
       <c r="M239" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N239" s="37"/>
@@ -11848,7 +11926,7 @@
         <v/>
       </c>
       <c r="M240" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N240" s="37"/>
@@ -11875,7 +11953,7 @@
         <v/>
       </c>
       <c r="M241" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N241" s="37"/>
@@ -11902,7 +11980,7 @@
         <v/>
       </c>
       <c r="M242" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N242" s="37"/>
@@ -11929,7 +12007,7 @@
         <v/>
       </c>
       <c r="M243" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N243" s="37"/>
@@ -11956,7 +12034,7 @@
         <v/>
       </c>
       <c r="M244" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N244" s="37"/>
@@ -11983,7 +12061,7 @@
         <v/>
       </c>
       <c r="M245" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N245" s="37"/>
@@ -12010,7 +12088,7 @@
         <v/>
       </c>
       <c r="M246" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N246" s="37"/>
@@ -12037,7 +12115,7 @@
         <v/>
       </c>
       <c r="M247" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N247" s="37"/>
@@ -12064,7 +12142,7 @@
         <v/>
       </c>
       <c r="M248" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N248" s="37"/>
@@ -12091,7 +12169,7 @@
         <v/>
       </c>
       <c r="M249" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N249" s="37"/>
@@ -12118,7 +12196,7 @@
         <v/>
       </c>
       <c r="M250" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N250" s="37"/>
@@ -12145,7 +12223,7 @@
         <v/>
       </c>
       <c r="M251" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N251" s="37"/>
@@ -12172,7 +12250,7 @@
         <v/>
       </c>
       <c r="M252" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N252" s="37"/>
@@ -12199,7 +12277,7 @@
         <v/>
       </c>
       <c r="M253" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N253" s="37"/>
@@ -12226,7 +12304,7 @@
         <v/>
       </c>
       <c r="M254" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N254" s="37"/>
@@ -12253,7 +12331,7 @@
         <v/>
       </c>
       <c r="M255" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N255" s="37"/>
@@ -12280,7 +12358,7 @@
         <v/>
       </c>
       <c r="M256" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N256" s="37"/>
@@ -12307,7 +12385,7 @@
         <v/>
       </c>
       <c r="M257" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N257" s="37"/>
@@ -12334,7 +12412,7 @@
         <v/>
       </c>
       <c r="M258" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N258" s="37"/>
@@ -12361,7 +12439,7 @@
         <v/>
       </c>
       <c r="M259" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N259" s="37"/>
@@ -12388,7 +12466,7 @@
         <v/>
       </c>
       <c r="M260" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N260" s="37"/>
@@ -12415,7 +12493,7 @@
         <v/>
       </c>
       <c r="M261" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N261" s="37"/>
@@ -12442,7 +12520,7 @@
         <v/>
       </c>
       <c r="M262" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N262" s="37"/>
@@ -12469,7 +12547,7 @@
         <v/>
       </c>
       <c r="M263" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N263" s="37"/>
@@ -12496,7 +12574,7 @@
         <v/>
       </c>
       <c r="M264" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N264" s="37"/>
@@ -12523,7 +12601,7 @@
         <v/>
       </c>
       <c r="M265" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N265" s="37"/>
@@ -12550,7 +12628,7 @@
         <v/>
       </c>
       <c r="M266" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N266" s="37"/>
@@ -12577,7 +12655,7 @@
         <v/>
       </c>
       <c r="M267" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N267" s="37"/>
@@ -12604,7 +12682,7 @@
         <v/>
       </c>
       <c r="M268" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N268" s="37"/>
@@ -12631,7 +12709,7 @@
         <v/>
       </c>
       <c r="M269" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N269" s="37"/>
@@ -12658,7 +12736,7 @@
         <v/>
       </c>
       <c r="M270" s="44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="M270:M333" si="16">IF(OR($C$6="",$C$7=""),"",IF(O270&lt;&gt;"",O270,IF(ISNUMBER(MATCH(N270,Q$2:Q$8,0)),N270,L270)))</f>
         <v/>
       </c>
       <c r="N270" s="37"/>
@@ -13036,7 +13114,7 @@
         <v/>
       </c>
       <c r="M284" s="44" t="str">
-        <f t="shared" ref="M284:M347" si="19">IF(OR($C$6="",$C$7=""),"",IF(O284&lt;&gt;"",O284,IF(N284="ED",N284,IF(N284="NS",N284,L284))))</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N284" s="37"/>
@@ -13063,7 +13141,7 @@
         <v/>
       </c>
       <c r="M285" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N285" s="37"/>
@@ -13090,7 +13168,7 @@
         <v/>
       </c>
       <c r="M286" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N286" s="37"/>
@@ -13117,7 +13195,7 @@
         <v/>
       </c>
       <c r="M287" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N287" s="37"/>
@@ -13144,7 +13222,7 @@
         <v/>
       </c>
       <c r="M288" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N288" s="37"/>
@@ -13171,7 +13249,7 @@
         <v/>
       </c>
       <c r="M289" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N289" s="37"/>
@@ -13198,7 +13276,7 @@
         <v/>
       </c>
       <c r="M290" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N290" s="37"/>
@@ -13225,7 +13303,7 @@
         <v/>
       </c>
       <c r="M291" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N291" s="37"/>
@@ -13252,7 +13330,7 @@
         <v/>
       </c>
       <c r="M292" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N292" s="37"/>
@@ -13279,7 +13357,7 @@
         <v/>
       </c>
       <c r="M293" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N293" s="37"/>
@@ -13306,7 +13384,7 @@
         <v/>
       </c>
       <c r="M294" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N294" s="37"/>
@@ -13333,7 +13411,7 @@
         <v/>
       </c>
       <c r="M295" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N295" s="37"/>
@@ -13360,7 +13438,7 @@
         <v/>
       </c>
       <c r="M296" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N296" s="37"/>
@@ -13387,7 +13465,7 @@
         <v/>
       </c>
       <c r="M297" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N297" s="37"/>
@@ -13414,7 +13492,7 @@
         <v/>
       </c>
       <c r="M298" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N298" s="37"/>
@@ -13441,7 +13519,7 @@
         <v/>
       </c>
       <c r="M299" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N299" s="37"/>
@@ -13468,7 +13546,7 @@
         <v/>
       </c>
       <c r="M300" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N300" s="37"/>
@@ -13495,7 +13573,7 @@
         <v/>
       </c>
       <c r="M301" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N301" s="37"/>
@@ -13522,7 +13600,7 @@
         <v/>
       </c>
       <c r="M302" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N302" s="37"/>
@@ -13549,7 +13627,7 @@
         <v/>
       </c>
       <c r="M303" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N303" s="37"/>
@@ -13576,7 +13654,7 @@
         <v/>
       </c>
       <c r="M304" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N304" s="37"/>
@@ -13603,7 +13681,7 @@
         <v/>
       </c>
       <c r="M305" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N305" s="37"/>
@@ -13630,7 +13708,7 @@
         <v/>
       </c>
       <c r="M306" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N306" s="37"/>
@@ -13657,7 +13735,7 @@
         <v/>
       </c>
       <c r="M307" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N307" s="37"/>
@@ -13684,7 +13762,7 @@
         <v/>
       </c>
       <c r="M308" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N308" s="37"/>
@@ -13711,7 +13789,7 @@
         <v/>
       </c>
       <c r="M309" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N309" s="37"/>
@@ -13738,7 +13816,7 @@
         <v/>
       </c>
       <c r="M310" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N310" s="37"/>
@@ -13765,7 +13843,7 @@
         <v/>
       </c>
       <c r="M311" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N311" s="37"/>
@@ -13792,7 +13870,7 @@
         <v/>
       </c>
       <c r="M312" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N312" s="37"/>
@@ -13819,7 +13897,7 @@
         <v/>
       </c>
       <c r="M313" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N313" s="37"/>
@@ -13846,7 +13924,7 @@
         <v/>
       </c>
       <c r="M314" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N314" s="37"/>
@@ -13873,7 +13951,7 @@
         <v/>
       </c>
       <c r="M315" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N315" s="37"/>
@@ -13900,7 +13978,7 @@
         <v/>
       </c>
       <c r="M316" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N316" s="37"/>
@@ -13927,7 +14005,7 @@
         <v/>
       </c>
       <c r="M317" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N317" s="37"/>
@@ -13954,7 +14032,7 @@
         <v/>
       </c>
       <c r="M318" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N318" s="37"/>
@@ -13981,7 +14059,7 @@
         <v/>
       </c>
       <c r="M319" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N319" s="37"/>
@@ -14008,7 +14086,7 @@
         <v/>
       </c>
       <c r="M320" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N320" s="37"/>
@@ -14035,7 +14113,7 @@
         <v/>
       </c>
       <c r="M321" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N321" s="37"/>
@@ -14062,7 +14140,7 @@
         <v/>
       </c>
       <c r="M322" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N322" s="37"/>
@@ -14089,7 +14167,7 @@
         <v/>
       </c>
       <c r="M323" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N323" s="37"/>
@@ -14116,7 +14194,7 @@
         <v/>
       </c>
       <c r="M324" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N324" s="37"/>
@@ -14143,7 +14221,7 @@
         <v/>
       </c>
       <c r="M325" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N325" s="37"/>
@@ -14170,7 +14248,7 @@
         <v/>
       </c>
       <c r="M326" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N326" s="37"/>
@@ -14197,7 +14275,7 @@
         <v/>
       </c>
       <c r="M327" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N327" s="37"/>
@@ -14224,7 +14302,7 @@
         <v/>
       </c>
       <c r="M328" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N328" s="37"/>
@@ -14251,7 +14329,7 @@
         <v/>
       </c>
       <c r="M329" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N329" s="37"/>
@@ -14278,7 +14356,7 @@
         <v/>
       </c>
       <c r="M330" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N330" s="37"/>
@@ -14305,7 +14383,7 @@
         <v/>
       </c>
       <c r="M331" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N331" s="37"/>
@@ -14332,7 +14410,7 @@
         <v/>
       </c>
       <c r="M332" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N332" s="37"/>
@@ -14359,7 +14437,7 @@
         <v/>
       </c>
       <c r="M333" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N333" s="37"/>
@@ -14386,7 +14464,7 @@
         <v/>
       </c>
       <c r="M334" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="M334:M397" si="19">IF(OR($C$6="",$C$7=""),"",IF(O334&lt;&gt;"",O334,IF(ISNUMBER(MATCH(N334,Q$2:Q$8,0)),N334,L334)))</f>
         <v/>
       </c>
       <c r="N334" s="37"/>
@@ -14764,7 +14842,7 @@
         <v/>
       </c>
       <c r="M348" s="44" t="str">
-        <f t="shared" ref="M348:M411" si="22">IF(OR($C$6="",$C$7=""),"",IF(O348&lt;&gt;"",O348,IF(N348="ED",N348,IF(N348="NS",N348,L348))))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N348" s="37"/>
@@ -14791,7 +14869,7 @@
         <v/>
       </c>
       <c r="M349" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N349" s="37"/>
@@ -14818,7 +14896,7 @@
         <v/>
       </c>
       <c r="M350" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N350" s="37"/>
@@ -14845,7 +14923,7 @@
         <v/>
       </c>
       <c r="M351" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N351" s="37"/>
@@ -14872,7 +14950,7 @@
         <v/>
       </c>
       <c r="M352" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N352" s="37"/>
@@ -14899,7 +14977,7 @@
         <v/>
       </c>
       <c r="M353" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N353" s="37"/>
@@ -14926,7 +15004,7 @@
         <v/>
       </c>
       <c r="M354" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N354" s="37"/>
@@ -14953,7 +15031,7 @@
         <v/>
       </c>
       <c r="M355" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N355" s="37"/>
@@ -14980,7 +15058,7 @@
         <v/>
       </c>
       <c r="M356" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N356" s="37"/>
@@ -15007,7 +15085,7 @@
         <v/>
       </c>
       <c r="M357" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N357" s="37"/>
@@ -15034,7 +15112,7 @@
         <v/>
       </c>
       <c r="M358" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N358" s="37"/>
@@ -15061,7 +15139,7 @@
         <v/>
       </c>
       <c r="M359" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N359" s="37"/>
@@ -15088,7 +15166,7 @@
         <v/>
       </c>
       <c r="M360" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N360" s="37"/>
@@ -15115,7 +15193,7 @@
         <v/>
       </c>
       <c r="M361" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N361" s="37"/>
@@ -15142,7 +15220,7 @@
         <v/>
       </c>
       <c r="M362" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N362" s="37"/>
@@ -15169,7 +15247,7 @@
         <v/>
       </c>
       <c r="M363" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N363" s="37"/>
@@ -15196,7 +15274,7 @@
         <v/>
       </c>
       <c r="M364" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N364" s="37"/>
@@ -15223,7 +15301,7 @@
         <v/>
       </c>
       <c r="M365" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N365" s="37"/>
@@ -15250,7 +15328,7 @@
         <v/>
       </c>
       <c r="M366" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N366" s="37"/>
@@ -15277,7 +15355,7 @@
         <v/>
       </c>
       <c r="M367" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N367" s="37"/>
@@ -15304,7 +15382,7 @@
         <v/>
       </c>
       <c r="M368" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N368" s="37"/>
@@ -15331,7 +15409,7 @@
         <v/>
       </c>
       <c r="M369" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N369" s="37"/>
@@ -15358,7 +15436,7 @@
         <v/>
       </c>
       <c r="M370" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N370" s="37"/>
@@ -15385,7 +15463,7 @@
         <v/>
       </c>
       <c r="M371" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N371" s="37"/>
@@ -15412,7 +15490,7 @@
         <v/>
       </c>
       <c r="M372" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N372" s="37"/>
@@ -15439,7 +15517,7 @@
         <v/>
       </c>
       <c r="M373" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N373" s="37"/>
@@ -15466,7 +15544,7 @@
         <v/>
       </c>
       <c r="M374" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N374" s="37"/>
@@ -15493,7 +15571,7 @@
         <v/>
       </c>
       <c r="M375" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N375" s="37"/>
@@ -15520,7 +15598,7 @@
         <v/>
       </c>
       <c r="M376" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N376" s="37"/>
@@ -15547,7 +15625,7 @@
         <v/>
       </c>
       <c r="M377" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N377" s="37"/>
@@ -15574,7 +15652,7 @@
         <v/>
       </c>
       <c r="M378" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N378" s="37"/>
@@ -15601,7 +15679,7 @@
         <v/>
       </c>
       <c r="M379" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N379" s="37"/>
@@ -15628,7 +15706,7 @@
         <v/>
       </c>
       <c r="M380" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N380" s="37"/>
@@ -15655,7 +15733,7 @@
         <v/>
       </c>
       <c r="M381" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N381" s="37"/>
@@ -15682,7 +15760,7 @@
         <v/>
       </c>
       <c r="M382" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N382" s="37"/>
@@ -15709,7 +15787,7 @@
         <v/>
       </c>
       <c r="M383" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N383" s="37"/>
@@ -15736,7 +15814,7 @@
         <v/>
       </c>
       <c r="M384" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N384" s="37"/>
@@ -15763,7 +15841,7 @@
         <v/>
       </c>
       <c r="M385" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N385" s="37"/>
@@ -15790,7 +15868,7 @@
         <v/>
       </c>
       <c r="M386" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N386" s="37"/>
@@ -15817,7 +15895,7 @@
         <v/>
       </c>
       <c r="M387" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N387" s="37"/>
@@ -15844,7 +15922,7 @@
         <v/>
       </c>
       <c r="M388" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N388" s="37"/>
@@ -15871,7 +15949,7 @@
         <v/>
       </c>
       <c r="M389" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N389" s="37"/>
@@ -15898,7 +15976,7 @@
         <v/>
       </c>
       <c r="M390" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N390" s="37"/>
@@ -15925,7 +16003,7 @@
         <v/>
       </c>
       <c r="M391" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N391" s="37"/>
@@ -15952,7 +16030,7 @@
         <v/>
       </c>
       <c r="M392" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N392" s="37"/>
@@ -15979,7 +16057,7 @@
         <v/>
       </c>
       <c r="M393" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N393" s="37"/>
@@ -16006,7 +16084,7 @@
         <v/>
       </c>
       <c r="M394" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N394" s="37"/>
@@ -16033,7 +16111,7 @@
         <v/>
       </c>
       <c r="M395" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N395" s="37"/>
@@ -16060,7 +16138,7 @@
         <v/>
       </c>
       <c r="M396" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N396" s="37"/>
@@ -16087,7 +16165,7 @@
         <v/>
       </c>
       <c r="M397" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N397" s="37"/>
@@ -16114,7 +16192,7 @@
         <v/>
       </c>
       <c r="M398" s="44" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="M398:M461" si="22">IF(OR($C$6="",$C$7=""),"",IF(O398&lt;&gt;"",O398,IF(ISNUMBER(MATCH(N398,Q$2:Q$8,0)),N398,L398)))</f>
         <v/>
       </c>
       <c r="N398" s="37"/>
@@ -16492,7 +16570,7 @@
         <v/>
       </c>
       <c r="M412" s="44" t="str">
-        <f t="shared" ref="M412:M475" si="25">IF(OR($C$6="",$C$7=""),"",IF(O412&lt;&gt;"",O412,IF(N412="ED",N412,IF(N412="NS",N412,L412))))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N412" s="37"/>
@@ -16519,7 +16597,7 @@
         <v/>
       </c>
       <c r="M413" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N413" s="37"/>
@@ -16546,7 +16624,7 @@
         <v/>
       </c>
       <c r="M414" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N414" s="37"/>
@@ -16573,7 +16651,7 @@
         <v/>
       </c>
       <c r="M415" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N415" s="37"/>
@@ -16600,7 +16678,7 @@
         <v/>
       </c>
       <c r="M416" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N416" s="37"/>
@@ -16627,7 +16705,7 @@
         <v/>
       </c>
       <c r="M417" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N417" s="37"/>
@@ -16654,7 +16732,7 @@
         <v/>
       </c>
       <c r="M418" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N418" s="37"/>
@@ -16681,7 +16759,7 @@
         <v/>
       </c>
       <c r="M419" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N419" s="37"/>
@@ -16708,7 +16786,7 @@
         <v/>
       </c>
       <c r="M420" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N420" s="37"/>
@@ -16735,7 +16813,7 @@
         <v/>
       </c>
       <c r="M421" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N421" s="37"/>
@@ -16762,7 +16840,7 @@
         <v/>
       </c>
       <c r="M422" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N422" s="37"/>
@@ -16789,7 +16867,7 @@
         <v/>
       </c>
       <c r="M423" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N423" s="37"/>
@@ -16816,7 +16894,7 @@
         <v/>
       </c>
       <c r="M424" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N424" s="37"/>
@@ -16843,7 +16921,7 @@
         <v/>
       </c>
       <c r="M425" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N425" s="37"/>
@@ -16870,7 +16948,7 @@
         <v/>
       </c>
       <c r="M426" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N426" s="37"/>
@@ -16897,7 +16975,7 @@
         <v/>
       </c>
       <c r="M427" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N427" s="37"/>
@@ -16924,7 +17002,7 @@
         <v/>
       </c>
       <c r="M428" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N428" s="37"/>
@@ -16951,7 +17029,7 @@
         <v/>
       </c>
       <c r="M429" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N429" s="37"/>
@@ -16978,7 +17056,7 @@
         <v/>
       </c>
       <c r="M430" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N430" s="37"/>
@@ -17005,7 +17083,7 @@
         <v/>
       </c>
       <c r="M431" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N431" s="37"/>
@@ -17032,7 +17110,7 @@
         <v/>
       </c>
       <c r="M432" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N432" s="37"/>
@@ -17059,7 +17137,7 @@
         <v/>
       </c>
       <c r="M433" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N433" s="37"/>
@@ -17086,7 +17164,7 @@
         <v/>
       </c>
       <c r="M434" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N434" s="37"/>
@@ -17113,7 +17191,7 @@
         <v/>
       </c>
       <c r="M435" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N435" s="37"/>
@@ -17140,7 +17218,7 @@
         <v/>
       </c>
       <c r="M436" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N436" s="37"/>
@@ -17167,7 +17245,7 @@
         <v/>
       </c>
       <c r="M437" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N437" s="37"/>
@@ -17194,7 +17272,7 @@
         <v/>
       </c>
       <c r="M438" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N438" s="37"/>
@@ -17221,7 +17299,7 @@
         <v/>
       </c>
       <c r="M439" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N439" s="37"/>
@@ -17248,7 +17326,7 @@
         <v/>
       </c>
       <c r="M440" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N440" s="37"/>
@@ -17275,7 +17353,7 @@
         <v/>
       </c>
       <c r="M441" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N441" s="37"/>
@@ -17302,7 +17380,7 @@
         <v/>
       </c>
       <c r="M442" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N442" s="37"/>
@@ -17329,7 +17407,7 @@
         <v/>
       </c>
       <c r="M443" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N443" s="37"/>
@@ -17356,7 +17434,7 @@
         <v/>
       </c>
       <c r="M444" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N444" s="37"/>
@@ -17383,7 +17461,7 @@
         <v/>
       </c>
       <c r="M445" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N445" s="37"/>
@@ -17410,7 +17488,7 @@
         <v/>
       </c>
       <c r="M446" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N446" s="37"/>
@@ -17437,7 +17515,7 @@
         <v/>
       </c>
       <c r="M447" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N447" s="37"/>
@@ -17464,7 +17542,7 @@
         <v/>
       </c>
       <c r="M448" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N448" s="37"/>
@@ -17491,7 +17569,7 @@
         <v/>
       </c>
       <c r="M449" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N449" s="37"/>
@@ -17518,7 +17596,7 @@
         <v/>
       </c>
       <c r="M450" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N450" s="37"/>
@@ -17545,7 +17623,7 @@
         <v/>
       </c>
       <c r="M451" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N451" s="37"/>
@@ -17572,7 +17650,7 @@
         <v/>
       </c>
       <c r="M452" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N452" s="37"/>
@@ -17599,7 +17677,7 @@
         <v/>
       </c>
       <c r="M453" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N453" s="37"/>
@@ -17626,7 +17704,7 @@
         <v/>
       </c>
       <c r="M454" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N454" s="37"/>
@@ -17653,7 +17731,7 @@
         <v/>
       </c>
       <c r="M455" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N455" s="37"/>
@@ -17680,7 +17758,7 @@
         <v/>
       </c>
       <c r="M456" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N456" s="37"/>
@@ -17707,7 +17785,7 @@
         <v/>
       </c>
       <c r="M457" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N457" s="37"/>
@@ -17734,7 +17812,7 @@
         <v/>
       </c>
       <c r="M458" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N458" s="37"/>
@@ -17761,7 +17839,7 @@
         <v/>
       </c>
       <c r="M459" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N459" s="37"/>
@@ -17788,7 +17866,7 @@
         <v/>
       </c>
       <c r="M460" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N460" s="37"/>
@@ -17815,7 +17893,7 @@
         <v/>
       </c>
       <c r="M461" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N461" s="37"/>
@@ -17842,7 +17920,7 @@
         <v/>
       </c>
       <c r="M462" s="44" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="M462:M513" si="25">IF(OR($C$6="",$C$7=""),"",IF(O462&lt;&gt;"",O462,IF(ISNUMBER(MATCH(N462,Q$2:Q$8,0)),N462,L462)))</f>
         <v/>
       </c>
       <c r="N462" s="37"/>
@@ -18220,7 +18298,7 @@
         <v/>
       </c>
       <c r="M476" s="44" t="str">
-        <f t="shared" ref="M476:M513" si="28">IF(OR($C$6="",$C$7=""),"",IF(O476&lt;&gt;"",O476,IF(N476="ED",N476,IF(N476="NS",N476,L476))))</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N476" s="37"/>
@@ -18247,7 +18325,7 @@
         <v/>
       </c>
       <c r="M477" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N477" s="37"/>
@@ -18274,7 +18352,7 @@
         <v/>
       </c>
       <c r="M478" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N478" s="37"/>
@@ -18301,7 +18379,7 @@
         <v/>
       </c>
       <c r="M479" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N479" s="37"/>
@@ -18328,7 +18406,7 @@
         <v/>
       </c>
       <c r="M480" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N480" s="37"/>
@@ -18355,7 +18433,7 @@
         <v/>
       </c>
       <c r="M481" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N481" s="37"/>
@@ -18382,7 +18460,7 @@
         <v/>
       </c>
       <c r="M482" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N482" s="37"/>
@@ -18409,7 +18487,7 @@
         <v/>
       </c>
       <c r="M483" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N483" s="37"/>
@@ -18436,7 +18514,7 @@
         <v/>
       </c>
       <c r="M484" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N484" s="37"/>
@@ -18463,7 +18541,7 @@
         <v/>
       </c>
       <c r="M485" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N485" s="37"/>
@@ -18490,7 +18568,7 @@
         <v/>
       </c>
       <c r="M486" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N486" s="37"/>
@@ -18517,7 +18595,7 @@
         <v/>
       </c>
       <c r="M487" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N487" s="37"/>
@@ -18544,7 +18622,7 @@
         <v/>
       </c>
       <c r="M488" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N488" s="37"/>
@@ -18571,7 +18649,7 @@
         <v/>
       </c>
       <c r="M489" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N489" s="37"/>
@@ -18598,7 +18676,7 @@
         <v/>
       </c>
       <c r="M490" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N490" s="37"/>
@@ -18625,7 +18703,7 @@
         <v/>
       </c>
       <c r="M491" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N491" s="37"/>
@@ -18652,7 +18730,7 @@
         <v/>
       </c>
       <c r="M492" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N492" s="37"/>
@@ -18679,7 +18757,7 @@
         <v/>
       </c>
       <c r="M493" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N493" s="37"/>
@@ -18706,7 +18784,7 @@
         <v/>
       </c>
       <c r="M494" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N494" s="37"/>
@@ -18733,7 +18811,7 @@
         <v/>
       </c>
       <c r="M495" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N495" s="37"/>
@@ -18760,7 +18838,7 @@
         <v/>
       </c>
       <c r="M496" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N496" s="37"/>
@@ -18787,7 +18865,7 @@
         <v/>
       </c>
       <c r="M497" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N497" s="37"/>
@@ -18814,7 +18892,7 @@
         <v/>
       </c>
       <c r="M498" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N498" s="37"/>
@@ -18841,7 +18919,7 @@
         <v/>
       </c>
       <c r="M499" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N499" s="37"/>
@@ -18868,7 +18946,7 @@
         <v/>
       </c>
       <c r="M500" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N500" s="37"/>
@@ -18895,7 +18973,7 @@
         <v/>
       </c>
       <c r="M501" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N501" s="37"/>
@@ -18922,7 +19000,7 @@
         <v/>
       </c>
       <c r="M502" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N502" s="37"/>
@@ -18949,7 +19027,7 @@
         <v/>
       </c>
       <c r="M503" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N503" s="37"/>
@@ -18976,7 +19054,7 @@
         <v/>
       </c>
       <c r="M504" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N504" s="37"/>
@@ -19003,7 +19081,7 @@
         <v/>
       </c>
       <c r="M505" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N505" s="37"/>
@@ -19030,7 +19108,7 @@
         <v/>
       </c>
       <c r="M506" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N506" s="37"/>
@@ -19057,7 +19135,7 @@
         <v/>
       </c>
       <c r="M507" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N507" s="37"/>
@@ -19084,7 +19162,7 @@
         <v/>
       </c>
       <c r="M508" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N508" s="37"/>
@@ -19111,7 +19189,7 @@
         <v/>
       </c>
       <c r="M509" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N509" s="37"/>
@@ -19138,7 +19216,7 @@
         <v/>
       </c>
       <c r="M510" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N510" s="37"/>
@@ -19165,7 +19243,7 @@
         <v/>
       </c>
       <c r="M511" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N511" s="37"/>
@@ -19192,7 +19270,7 @@
         <v/>
       </c>
       <c r="M512" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N512" s="37"/>
@@ -19219,7 +19297,7 @@
         <v/>
       </c>
       <c r="M513" s="44" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="N513" s="37"/>
@@ -19236,6 +19314,14 @@
       <sortCondition ref="K12"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.43307086614173229" right="0.47244094488188981" top="0.6692913385826772" bottom="0.55118110236220474" header="0.51181102362204722" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" firstPageNumber="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -19298,21 +19384,21 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.15">
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
@@ -19320,23 +19406,23 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
         <v>53</v>
-      </c>
-      <c r="E7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.15">
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.15">
@@ -19344,7 +19430,7 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.15">
@@ -19352,7 +19438,7 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.15">
@@ -19360,7 +19446,7 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.15">
@@ -19368,12 +19454,12 @@
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.15">
@@ -19386,18 +19472,18 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
         <v>61</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.15">
@@ -19407,57 +19493,57 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.15">
@@ -19467,7 +19553,7 @@
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -19477,6 +19563,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060D23BF17FCDC947B8E404D646247F8D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f8a301bd3e0c8b5ed750a66ab7022">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0f5e39c8-e5a1-4a0d-b53f-9134be983d19" xmlns:ns3="c64b295e-e158-430a-a9fe-95bbf17b9d7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="765cdbe449e857445462344bdfd818c7" ns2:_="" ns3:_="">
     <xsd:import namespace="0f5e39c8-e5a1-4a0d-b53f-9134be983d19"/>
@@ -19693,22 +19788,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB09DFA-8D31-49CC-B484-1597D6808628}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A6C0948-47EA-46A4-908A-6D65E67CB754}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19727,7 +19821,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5FF57B8-CD17-4BF7-BF02-BCE169B04897}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -19742,12 +19836,4 @@
     <ds:schemaRef ds:uri="0f5e39c8-e5a1-4a0d-b53f-9134be983d19"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB09DFA-8D31-49CC-B484-1597D6808628}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update a bunch of stuff :)
</commit_message>
<xml_diff>
--- a/data/subject_results/Blank-Results.xlsx
+++ b/data/subject_results/Blank-Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sci-lmw1/dev/HelpLindsay/data/subject_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA6B923-A54E-EB41-89B9-DFDF3F96965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F8E35-7CD0-FA4B-907A-5FD8D14E95BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22060" windowHeight="17340" tabRatio="519" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="22060" windowHeight="17340" tabRatio="519" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StudentOne" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>Study Period</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>A1</t>
+  </si>
+  <si>
+    <t>Lindsay Ward</t>
   </si>
 </sst>
 </file>
@@ -1381,11 +1384,11 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1407,20 +1410,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1449,8 +1438,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="7"/>
-      <tableStyleElement type="headerRow" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -6652,7 +6641,7 @@
       <selection activeCell="R15" sqref="R15"/>
       <selection pane="topRight" activeCell="R15" sqref="R15"/>
       <selection pane="bottomLeft" activeCell="R15" sqref="R15"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6938,11 +6927,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="57"/>
+      <c r="C7" s="57" t="s">
+        <v>61</v>
+      </c>
       <c r="E7" s="66" t="s">
         <v>59</v>
       </c>
@@ -6964,13 +6955,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="57"/>
+      <c r="C8" s="57" t="s">
+        <v>61</v>
+      </c>
       <c r="E8" s="70" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -14485,34 +14478,24 @@
     <protectedRange sqref="A12:P199" name="Range1"/>
   </protectedRanges>
   <autoFilter ref="A12:P199" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="notEqual">
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+  <conditionalFormatting sqref="C7:C8">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
-      <formula>""</formula>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
-      <formula>""</formula>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -14545,26 +14528,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c64b295e-e158-430a-a9fe-95bbf17b9d7d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0f5e39c8-e5a1-4a0d-b53f-9134be983d19">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060D23BF17FCDC947B8E404D646247F8D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29d8ace8dc41074792c1ec8140cc849b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0f5e39c8-e5a1-4a0d-b53f-9134be983d19" xmlns:ns3="c64b295e-e158-430a-a9fe-95bbf17b9d7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f469e829c8e0d9e5502ef49b41822689" ns2:_="" ns3:_="">
     <xsd:import namespace="0f5e39c8-e5a1-4a0d-b53f-9134be983d19"/>
@@ -14807,10 +14770,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c64b295e-e158-430a-a9fe-95bbf17b9d7d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0f5e39c8-e5a1-4a0d-b53f-9134be983d19">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB09DFA-8D31-49CC-B484-1597D6808628}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0143DE52-0693-4E7D-AE2A-7F5F78F30281}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0f5e39c8-e5a1-4a0d-b53f-9134be983d19"/>
+    <ds:schemaRef ds:uri="c64b295e-e158-430a-a9fe-95bbf17b9d7d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14833,20 +14827,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0143DE52-0693-4E7D-AE2A-7F5F78F30281}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB09DFA-8D31-49CC-B484-1597D6808628}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0f5e39c8-e5a1-4a0d-b53f-9134be983d19"/>
-    <ds:schemaRef ds:uri="c64b295e-e158-430a-a9fe-95bbf17b9d7d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>